<commit_message>
Made nnMakeArray skip empty strings.
</commit_message>
<xml_diff>
--- a/Samples/Iris-flower-data-set.xlsx
+++ b/Samples/Iris-flower-data-set.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -604,7 +604,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S152"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -718,15 +718,15 @@
       </c>
       <c r="M3" s="23">
         <f t="array" aca="1" ref="M3:O3" ca="1">_xll.nnFeedForward($K$20,A3:D3)</f>
-        <v>7.7114666530281764E-6</v>
+        <v>1.3735626106854686E-5</v>
       </c>
       <c r="N3" s="23">
         <f ca="1"/>
-        <v>2.5033582778322015E-3</v>
+        <v>6.1703230831915788E-3</v>
       </c>
       <c r="O3" s="23">
         <f ca="1"/>
-        <v>0.99748893025551477</v>
+        <v>0.99381594129070161</v>
       </c>
       <c r="P3" s="4">
         <f ca="1">IF(M3=MAX($M3:$O3),1,0)</f>
@@ -742,7 +742,7 @@
       </c>
       <c r="S3" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F3:H3,M3:O3)</f>
-        <v>2.5142277679018506E-3</v>
+        <v>6.2032591992580641E-3</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -770,15 +770,15 @@
       </c>
       <c r="M4" s="23">
         <f t="array" aca="1" ref="M4:O4" ca="1">_xll.nnFeedForward($K$20,A4:D4)</f>
-        <v>6.5500434031278386E-4</v>
+        <v>1.1278449126143513E-3</v>
       </c>
       <c r="N4" s="23">
         <f ca="1"/>
-        <v>0.98615074397813141</v>
+        <v>0.97460754882109535</v>
       </c>
       <c r="O4" s="23">
         <f ca="1"/>
-        <v>1.3194251681555908E-2</v>
+        <v>2.4264606266290324E-2</v>
       </c>
       <c r="P4" s="4">
         <f t="shared" ref="P4:P67" ca="1" si="1">IF(M4=MAX($M4:$O4),1,0)</f>
@@ -794,7 +794,7 @@
       </c>
       <c r="S4" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F4:H4,M4:O4)</f>
-        <v>1.3946051705964616E-2</v>
+        <v>2.5720403044452379E-2</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -825,15 +825,15 @@
       </c>
       <c r="M5" s="23">
         <f t="array" aca="1" ref="M5:O5" ca="1">_xll.nnFeedForward($K$20,A5:D5)</f>
-        <v>7.3867363900383619E-4</v>
+        <v>1.276728284975117E-3</v>
       </c>
       <c r="N5" s="23">
         <f ca="1"/>
-        <v>0.9956341109113922</v>
+        <v>0.99612409125008572</v>
       </c>
       <c r="O5" s="23">
         <f ca="1"/>
-        <v>3.6272154496039179E-3</v>
+        <v>2.5991804649390937E-3</v>
       </c>
       <c r="P5" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -849,7 +849,7 @@
       </c>
       <c r="S5" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F5:H5,M5:O5)</f>
-        <v>4.3754474129093571E-3</v>
+        <v>3.8834395496597056E-3</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -883,15 +883,15 @@
       </c>
       <c r="M6" s="23">
         <f t="array" aca="1" ref="M6:O6" ca="1">_xll.nnFeedForward($K$20,A6:D6)</f>
-        <v>7.679189774104421E-6</v>
+        <v>5.3697743741959384E-6</v>
       </c>
       <c r="N6" s="23">
         <f ca="1"/>
-        <v>2.491897351934903E-3</v>
+        <v>2.1139522562891116E-3</v>
       </c>
       <c r="O6" s="23">
         <f ca="1"/>
-        <v>0.99750042345829093</v>
+        <v>0.99788067796933666</v>
       </c>
       <c r="P6" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -907,7 +907,7 @@
       </c>
       <c r="S6" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F6:H6,M6:O6)</f>
-        <v>2.5027056986187341E-3</v>
+        <v>2.1215709716467602E-3</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -941,15 +941,15 @@
       </c>
       <c r="M7" s="23">
         <f t="array" aca="1" ref="M7:O7" ca="1">_xll.nnFeedForward($K$20,A7:D7)</f>
-        <v>7.7855957858453608E-6</v>
+        <v>6.1687280717749319E-5</v>
       </c>
       <c r="N7" s="23">
         <f ca="1"/>
-        <v>2.5331685289527528E-3</v>
+        <v>3.1892987007182037E-2</v>
       </c>
       <c r="O7" s="23">
         <f ca="1"/>
-        <v>0.99745904587526146</v>
+        <v>0.96804532571210011</v>
       </c>
       <c r="P7" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -965,7 +965,7 @@
       </c>
       <c r="S7" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F7:H7,M7:O7)</f>
-        <v>2.5441878276258193E-3</v>
+        <v>3.247636871902513E-2</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -999,15 +999,15 @@
       </c>
       <c r="M8" s="23">
         <f t="array" aca="1" ref="M8:O8" ca="1">_xll.nnFeedForward($K$20,A8:D8)</f>
-        <v>8.2678983304314627E-4</v>
+        <v>1.3154483782248526E-3</v>
       </c>
       <c r="N8" s="23">
         <f ca="1"/>
-        <v>0.99585152439230307</v>
+        <v>0.99628392531818588</v>
       </c>
       <c r="O8" s="23">
         <f ca="1"/>
-        <v>3.3216857746538081E-3</v>
+        <v>2.400626303589178E-3</v>
       </c>
       <c r="P8" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -1023,7 +1023,7 @@
       </c>
       <c r="S8" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F8:H8,M8:O8)</f>
-        <v>4.1571044051362145E-3</v>
+        <v>3.7229964405034481E-3</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -1057,15 +1057,15 @@
       </c>
       <c r="M9" s="23">
         <f t="array" aca="1" ref="M9:O9" ca="1">_xll.nnFeedForward($K$20,A9:D9)</f>
-        <v>0.99888856757764888</v>
+        <v>0.99883448624878901</v>
       </c>
       <c r="N9" s="23">
         <f ca="1"/>
-        <v>1.1087998410992711E-3</v>
+        <v>1.162890823080678E-3</v>
       </c>
       <c r="O9" s="23">
         <f ca="1"/>
-        <v>2.6325812518823511E-6</v>
+        <v>2.6229281302756318E-6</v>
       </c>
       <c r="P9" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -1081,7 +1081,7 @@
       </c>
       <c r="S9" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F9:H9,M9:O9)</f>
-        <v>1.1120505213918345E-3</v>
+        <v>1.1661934905781704E-3</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -1115,15 +1115,15 @@
       </c>
       <c r="M10" s="23">
         <f t="array" aca="1" ref="M10:O10" ca="1">_xll.nnFeedForward($K$20,A10:D10)</f>
-        <v>8.4070387851131057E-6</v>
+        <v>5.1334712041849968E-5</v>
       </c>
       <c r="N10" s="23">
         <f ca="1"/>
-        <v>2.7606559408118927E-3</v>
+        <v>2.6571746449383208E-2</v>
       </c>
       <c r="O10" s="23">
         <f ca="1"/>
-        <v>0.997230937020403</v>
+        <v>0.97337691883857491</v>
       </c>
       <c r="P10" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -1139,7 +1139,7 @@
       </c>
       <c r="S10" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F10:H10,M10:O10)</f>
-        <v>2.7729039266776714E-3</v>
+        <v>2.6983893761824099E-2</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -1173,15 +1173,15 @@
       </c>
       <c r="M11" s="23">
         <f t="array" aca="1" ref="M11:O11" ca="1">_xll.nnFeedForward($K$20,A11:D11)</f>
-        <v>6.5159480926201268E-4</v>
+        <v>1.166235409178233E-3</v>
       </c>
       <c r="N11" s="23">
         <f ca="1"/>
-        <v>0.99449334932300948</v>
+        <v>0.99433388543528922</v>
       </c>
       <c r="O11" s="23">
         <f ca="1"/>
-        <v>4.8550558677283705E-3</v>
+        <v>4.4998791555325469E-3</v>
       </c>
       <c r="P11" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="S11" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F11:H11,M11:O11)</f>
-        <v>5.521868168480883E-3</v>
+        <v>5.6822278872890961E-3</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -1228,19 +1228,19 @@
       </c>
       <c r="K12" s="13">
         <f ca="1">RAND()*32000</f>
-        <v>23115.646378823996</v>
+        <v>30758.999259896773</v>
       </c>
       <c r="M12" s="23">
         <f t="array" aca="1" ref="M12:O12" ca="1">_xll.nnFeedForward($K$20,A12:D12)</f>
-        <v>7.6813901029703954E-6</v>
+        <v>9.623941845829908E-6</v>
       </c>
       <c r="N12" s="23">
         <f ca="1"/>
-        <v>2.4934027901826672E-3</v>
+        <v>4.1241662344473715E-3</v>
       </c>
       <c r="O12" s="23">
         <f ca="1"/>
-        <v>0.99749891581971439</v>
+        <v>0.99586620982370677</v>
       </c>
       <c r="P12" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="S12" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F12:H12,M12:O12)</f>
-        <v>2.5042171162386342E-3</v>
+        <v>4.1423579065217901E-3</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -1288,15 +1288,15 @@
       </c>
       <c r="M13" s="23">
         <f t="array" aca="1" ref="M13:O13" ca="1">_xll.nnFeedForward($K$20,A13:D13)</f>
-        <v>7.7372932081056042E-6</v>
+        <v>4.6308564645477758E-5</v>
       </c>
       <c r="N13" s="23">
         <f ca="1"/>
-        <v>2.5141560298309971E-3</v>
+        <v>2.349738463938375E-2</v>
       </c>
       <c r="O13" s="23">
         <f ca="1"/>
-        <v>0.99747810667696091</v>
+        <v>0.97645630679597073</v>
       </c>
       <c r="P13" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -1312,7 +1312,7 @@
       </c>
       <c r="S13" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F13:H13,M13:O13)</f>
-        <v>2.525078652506554E-3</v>
+        <v>2.3825274371064652E-2</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -1340,15 +1340,15 @@
       </c>
       <c r="M14" s="23">
         <f t="array" aca="1" ref="M14:O14" ca="1">_xll.nnFeedForward($K$20,A14:D14)</f>
-        <v>1.4964010426184436E-5</v>
+        <v>8.633033948319215E-5</v>
       </c>
       <c r="N14" s="23">
         <f ca="1"/>
-        <v>5.3174251238235068E-3</v>
+        <v>5.0925331200835332E-2</v>
       </c>
       <c r="O14" s="23">
         <f ca="1"/>
-        <v>0.99466761086575028</v>
+        <v>0.94898833845968156</v>
       </c>
       <c r="P14" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -1364,7 +1364,7 @@
       </c>
       <c r="S14" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F14:H14,M14:O14)</f>
-        <v>5.2367660920753387</v>
+        <v>2.9773948131921282</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -1395,15 +1395,15 @@
       </c>
       <c r="M15" s="23">
         <f t="array" aca="1" ref="M15:O15" ca="1">_xll.nnFeedForward($K$20,A15:D15)</f>
-        <v>0.99888139963552258</v>
+        <v>0.99883150317756098</v>
       </c>
       <c r="N15" s="23">
         <f ca="1"/>
-        <v>1.1159514143383369E-3</v>
+        <v>1.1658668143610465E-3</v>
       </c>
       <c r="O15" s="23">
         <f ca="1"/>
-        <v>2.6489501390034322E-6</v>
+        <v>2.6300080778782959E-6</v>
       </c>
       <c r="P15" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -1419,7 +1419,7 @@
       </c>
       <c r="S15" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F15:H15,M15:O15)</f>
-        <v>1.1192264648127138E-3</v>
+        <v>1.1691800471334975E-3</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -1453,15 +1453,15 @@
       </c>
       <c r="M16" s="23">
         <f t="array" aca="1" ref="M16:O16" ca="1">_xll.nnFeedForward($K$20,A16:D16)</f>
-        <v>7.6720317500125468E-6</v>
+        <v>1.1227419387813871E-5</v>
       </c>
       <c r="N16" s="23">
         <f ca="1"/>
-        <v>2.4904516291071885E-3</v>
+        <v>4.9112710019030507E-3</v>
       </c>
       <c r="O16" s="23">
         <f ca="1"/>
-        <v>0.99750187633914278</v>
+        <v>0.99507750157870922</v>
       </c>
       <c r="P16" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -1477,7 +1477,7 @@
       </c>
       <c r="S16" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F16:H16,M16:O16)</f>
-        <v>2.5012491781405402E-3</v>
+        <v>4.9346538230147325E-3</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
@@ -1512,15 +1512,15 @@
       </c>
       <c r="M17" s="23">
         <f t="array" aca="1" ref="M17:O17" ca="1">_xll.nnFeedForward($K$20,A17:D17)</f>
-        <v>7.6890370727888242E-6</v>
+        <v>2.4423480168810108E-5</v>
       </c>
       <c r="N17" s="23">
         <f ca="1"/>
-        <v>2.4960518986222812E-3</v>
+        <v>1.1721592630106938E-2</v>
       </c>
       <c r="O17" s="23">
         <f ca="1"/>
-        <v>0.99749625906430495</v>
+        <v>0.9882539838897243</v>
       </c>
       <c r="P17" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -1536,7 +1536,7 @@
       </c>
       <c r="S17" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F17:H17,M17:O17)</f>
-        <v>2.5068805366247038E-3</v>
+        <v>1.181554555647368E-2</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
@@ -1570,15 +1570,15 @@
       </c>
       <c r="M18" s="23">
         <f t="array" aca="1" ref="M18:O18" ca="1">_xll.nnFeedForward($K$20,A18:D18)</f>
-        <v>3.4713345901378122E-5</v>
+        <v>2.1967692752002257E-4</v>
       </c>
       <c r="N18" s="23">
         <f ca="1"/>
-        <v>1.3940092975885872E-2</v>
+        <v>0.14477969614226474</v>
       </c>
       <c r="O18" s="23">
         <f ca="1"/>
-        <v>0.98602519367821284</v>
+        <v>0.85500062693021517</v>
       </c>
       <c r="P18" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -1594,7 +1594,7 @@
       </c>
       <c r="S18" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F18:H18,M18:O18)</f>
-        <v>1.4073373308151253E-2</v>
+        <v>0.15665307679393201</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
@@ -1625,15 +1625,15 @@
       </c>
       <c r="M19" s="23">
         <f t="array" aca="1" ref="M19:O19" ca="1">_xll.nnFeedForward($K$20,A19:D19)</f>
-        <v>8.7539361740619277E-6</v>
+        <v>6.6668036262955562E-5</v>
       </c>
       <c r="N19" s="23">
         <f ca="1"/>
-        <v>2.891183963333886E-3</v>
+        <v>3.5198743846080051E-2</v>
       </c>
       <c r="O19" s="23">
         <f ca="1"/>
-        <v>0.99710006210049207</v>
+        <v>0.964734588117657</v>
       </c>
       <c r="P19" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -1649,7 +1649,7 @@
       </c>
       <c r="S19" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F19:H19,M19:O19)</f>
-        <v>2.9041508662844733E-3</v>
+        <v>3.5902253693143545E-2</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
@@ -1681,15 +1681,15 @@
       </c>
       <c r="M20" s="23">
         <f t="array" aca="1" ref="M20:O20" ca="1">_xll.nnFeedForward($K$20,A20:D20)</f>
-        <v>0.99890922481876188</v>
+        <v>0.99884650350284643</v>
       </c>
       <c r="N20" s="23">
         <f ca="1"/>
-        <v>1.0881911053104935E-3</v>
+        <v>1.1509014281717073E-3</v>
       </c>
       <c r="O20" s="23">
         <f ca="1"/>
-        <v>2.5840759275044132E-6</v>
+        <v>2.5950689819703965E-6</v>
       </c>
       <c r="P20" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -1705,7 +1705,7 @@
       </c>
       <c r="S20" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F20:H20,M20:O20)</f>
-        <v>1.0913705094383172E-3</v>
+        <v>1.1541622862775718E-3</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
@@ -1733,15 +1733,15 @@
       </c>
       <c r="M21" s="23">
         <f t="array" aca="1" ref="M21:O21" ca="1">_xll.nnFeedForward($K$20,A21:D21)</f>
-        <v>6.9280662015916926E-4</v>
+        <v>1.2649967514179949E-3</v>
       </c>
       <c r="N21" s="23">
         <f ca="1"/>
-        <v>0.99563036144457973</v>
+        <v>0.99615935985684156</v>
       </c>
       <c r="O21" s="23">
         <f ca="1"/>
-        <v>3.6768319352610598E-3</v>
+        <v>2.5756433917403965E-3</v>
       </c>
       <c r="P21" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -1757,7 +1757,7 @@
       </c>
       <c r="S21" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F21:H21,M21:O21)</f>
-        <v>4.3792133283510589E-3</v>
+        <v>3.8480343398840243E-3</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
@@ -1788,15 +1788,15 @@
       </c>
       <c r="M22" s="23">
         <f t="array" aca="1" ref="M22:O22" ca="1">_xll.nnFeedForward($K$20,A22:D22)</f>
-        <v>7.692693270668439E-6</v>
+        <v>9.1699255138426849E-6</v>
       </c>
       <c r="N22" s="23">
         <f ca="1"/>
-        <v>2.4968905250401549E-3</v>
+        <v>3.9016061626642728E-3</v>
       </c>
       <c r="O22" s="23">
         <f ca="1"/>
-        <v>0.99749541678168918</v>
+        <v>0.99608922391182186</v>
       </c>
       <c r="P22" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -1812,7 +1812,7 @@
       </c>
       <c r="S22" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F22:H22,M22:O22)</f>
-        <v>2.5077249337477222E-3</v>
+        <v>3.9184431690031307E-3</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
@@ -1843,19 +1843,19 @@
       </c>
       <c r="K23" s="12">
         <f ca="1">AVERAGE(S33:S152)</f>
-        <v>1.3535127168074588E-2</v>
+        <v>2.2913257365822361E-2</v>
       </c>
       <c r="M23" s="23">
         <f t="array" aca="1" ref="M23:O23" ca="1">_xll.nnFeedForward($K$20,A23:D23)</f>
-        <v>0.99885008658924324</v>
+        <v>0.99877718721897901</v>
       </c>
       <c r="N23" s="23">
         <f ca="1"/>
-        <v>1.1471659918669168E-3</v>
+        <v>1.2200565713065875E-3</v>
       </c>
       <c r="O23" s="23">
         <f ca="1"/>
-        <v>2.7474188897582965E-6</v>
+        <v>2.7562097144779043E-6</v>
       </c>
       <c r="P23" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -1871,7 +1871,7 @@
       </c>
       <c r="S23" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F23:H23,M23:O23)</f>
-        <v>1.1505750684642334E-3</v>
+        <v>1.2235610266080777E-3</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
@@ -1902,19 +1902,19 @@
       </c>
       <c r="K24" s="12">
         <f ca="1">AVERAGE(S3:S32)</f>
-        <v>0.53797699803240906</v>
+        <v>0.33888518517307847</v>
       </c>
       <c r="M24" s="23">
         <f t="array" aca="1" ref="M24:O24" ca="1">_xll.nnFeedForward($K$20,A24:D24)</f>
-        <v>1.8904902242697424E-5</v>
+        <v>8.0914328347672448E-5</v>
       </c>
       <c r="N24" s="23">
         <f ca="1"/>
-        <v>6.9263139159237101E-3</v>
+        <v>4.9765768957504418E-2</v>
       </c>
       <c r="O24" s="23">
         <f ca="1"/>
-        <v>0.99305478118183366</v>
+        <v>0.95015331671414782</v>
       </c>
       <c r="P24" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -1930,7 +1930,7 @@
       </c>
       <c r="S24" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F24:H24,M24:O24)</f>
-        <v>4.9724275097547341</v>
+        <v>3.0004279016300641</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
@@ -1961,19 +1961,19 @@
       </c>
       <c r="K25" s="10">
         <f ca="1">(SUMPRODUCT(F33:H152,P33:R152))/COUNTA(P33:P152)</f>
-        <v>0.9916666666666667</v>
+        <v>1</v>
       </c>
       <c r="M25" s="23">
         <f t="array" aca="1" ref="M25:O25" ca="1">_xll.nnFeedForward($K$20,A25:D25)</f>
-        <v>7.8135356096432238E-6</v>
+        <v>2.7464582212273926E-5</v>
       </c>
       <c r="N25" s="23">
         <f ca="1"/>
-        <v>2.5412809446430269E-3</v>
+        <v>1.3356378130589517E-2</v>
       </c>
       <c r="O25" s="23">
         <f ca="1"/>
-        <v>0.99745090551974724</v>
+        <v>0.9866161572871982</v>
       </c>
       <c r="P25" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -1989,7 +1989,7 @@
       </c>
       <c r="S25" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F25:H25,M25:O25)</f>
-        <v>2.5523489534035235E-3</v>
+        <v>1.3474213581143167E-2</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
@@ -2024,15 +2024,15 @@
       </c>
       <c r="M26" s="23">
         <f t="array" aca="1" ref="M26:O26" ca="1">_xll.nnFeedForward($K$20,A26:D26)</f>
-        <v>8.3157367234894383E-4</v>
+        <v>1.3828702757114166E-3</v>
       </c>
       <c r="N26" s="23">
         <f ca="1"/>
-        <v>0.99599902965753195</v>
+        <v>0.99642354642808739</v>
       </c>
       <c r="O26" s="23">
         <f ca="1"/>
-        <v>3.1693966701190441E-3</v>
+        <v>2.1935832962011719E-3</v>
       </c>
       <c r="P26" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -2048,7 +2048,7 @@
       </c>
       <c r="S26" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F26:H26,M26:O26)</f>
-        <v>4.0089956374391392E-3</v>
+        <v>3.5828643718384626E-3</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
@@ -2076,15 +2076,15 @@
       </c>
       <c r="M27" s="23">
         <f t="array" aca="1" ref="M27:O27" ca="1">_xll.nnFeedForward($K$20,A27:D27)</f>
-        <v>0.99884824290813856</v>
+        <v>0.99877633327769211</v>
       </c>
       <c r="N27" s="23">
         <f ca="1"/>
-        <v>1.1490075557351409E-3</v>
+        <v>1.2209086114696747E-3</v>
       </c>
       <c r="O27" s="23">
         <f ca="1"/>
-        <v>2.7495361262731017E-6</v>
+        <v>2.7581108381994911E-6</v>
       </c>
       <c r="P27" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -2100,7 +2100,7 @@
       </c>
       <c r="S27" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F27:H27,M27:O27)</f>
-        <v>1.1524208737867404E-3</v>
+        <v>1.2244160137492408E-3</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
@@ -2128,15 +2128,15 @@
       </c>
       <c r="M28" s="23">
         <f t="array" aca="1" ref="M28:O28" ca="1">_xll.nnFeedForward($K$20,A28:D28)</f>
-        <v>8.8972590199064295E-6</v>
+        <v>4.904198332906472E-5</v>
       </c>
       <c r="N28" s="23">
         <f ca="1"/>
-        <v>2.9428827127631367E-3</v>
+        <v>2.5520792406116748E-2</v>
       </c>
       <c r="O28" s="23">
         <f ca="1"/>
-        <v>0.99704822002821691</v>
+        <v>0.97443016561055418</v>
       </c>
       <c r="P28" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -2152,7 +2152,7 @@
       </c>
       <c r="S28" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F28:H28,M28:O28)</f>
-        <v>5.8283656634766547</v>
+        <v>3.6682617705911773</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
@@ -2180,15 +2180,15 @@
       </c>
       <c r="M29" s="23">
         <f t="array" aca="1" ref="M29:O29" ca="1">_xll.nnFeedForward($K$20,A29:D29)</f>
-        <v>8.4281644088461866E-4</v>
+        <v>1.3089063100652865E-3</v>
       </c>
       <c r="N29" s="23">
         <f ca="1"/>
-        <v>0.99578859967490485</v>
+        <v>0.99645354394045138</v>
       </c>
       <c r="O29" s="23">
         <f ca="1"/>
-        <v>3.3685838842106128E-3</v>
+        <v>2.2375497494834173E-3</v>
       </c>
       <c r="P29" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -2204,7 +2204,7 @@
       </c>
       <c r="S29" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F29:H29,M29:O29)</f>
-        <v>4.2202932479987014E-3</v>
+        <v>3.5527596428401413E-3</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
@@ -2232,15 +2232,15 @@
       </c>
       <c r="M30" s="23">
         <f t="array" aca="1" ref="M30:O30" ca="1">_xll.nnFeedForward($K$20,A30:D30)</f>
-        <v>0.99889394164076051</v>
+        <v>0.99882918586924352</v>
       </c>
       <c r="N30" s="23">
         <f ca="1"/>
-        <v>1.1034275843646085E-3</v>
+        <v>1.1681787399554873E-3</v>
       </c>
       <c r="O30" s="23">
         <f ca="1"/>
-        <v>2.6307748748626006E-6</v>
+        <v>2.6353908009995763E-6</v>
       </c>
       <c r="P30" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -2256,7 +2256,7 @@
       </c>
       <c r="S30" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F30:H30,M30:O30)</f>
-        <v>1.1066704931987307E-3</v>
+        <v>1.1715000690773276E-3</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
@@ -2284,15 +2284,15 @@
       </c>
       <c r="M31" s="23">
         <f t="array" aca="1" ref="M31:O31" ca="1">_xll.nnFeedForward($K$20,A31:D31)</f>
-        <v>0.99881604126233492</v>
+        <v>0.99874589336660025</v>
       </c>
       <c r="N31" s="23">
         <f ca="1"/>
-        <v>1.1811289828484693E-3</v>
+        <v>1.2512779608796929E-3</v>
       </c>
       <c r="O31" s="23">
         <f ca="1"/>
-        <v>2.8297548166318252E-6</v>
+        <v>2.8286725200778715E-6</v>
       </c>
       <c r="P31" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -2308,7 +2308,7 @@
       </c>
       <c r="S31" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F31:H31,M31:O31)</f>
-        <v>1.1846601705110176E-3</v>
+        <v>1.2548936832221407E-3</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
@@ -2342,15 +2342,15 @@
       <c r="L32" s="7"/>
       <c r="M32" s="24">
         <f t="array" aca="1" ref="M32:O32" ca="1">_xll.nnFeedForward($K$20,A32:D32)</f>
-        <v>2.7635006845044733E-5</v>
+        <v>2.0659637252960769E-4</v>
       </c>
       <c r="N32" s="24">
         <f ca="1"/>
-        <v>1.0729764728730481E-2</v>
+        <v>0.13014260286368379</v>
       </c>
       <c r="O32" s="24">
         <f ca="1"/>
-        <v>0.98924260026442445</v>
+        <v>0.86965080076378654</v>
       </c>
       <c r="P32" s="22">
         <f t="shared" ca="1" si="1"/>
@@ -2366,7 +2366,7 @@
       </c>
       <c r="S32" s="9">
         <f ca="1">_xll.nnGetCrossEntropyError(F32:H32,M32:O32)</f>
-        <v>1.0815678891737309E-2</v>
+        <v>0.13966352633982107</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
@@ -2397,15 +2397,15 @@
       </c>
       <c r="M33" s="23">
         <f t="array" aca="1" ref="M33:O33" ca="1">_xll.nnFeedForward($K$20,A33:D33)</f>
-        <v>7.6942745925589802E-6</v>
+        <v>7.6894838203931444E-6</v>
       </c>
       <c r="N33" s="23">
         <f ca="1"/>
-        <v>2.4967404240138166E-3</v>
+        <v>3.1929189101294101E-3</v>
       </c>
       <c r="O33" s="23">
         <f ca="1"/>
-        <v>0.99749556530139361</v>
+        <v>0.99679939160605024</v>
       </c>
       <c r="P33" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -2421,7 +2421,7 @@
       </c>
       <c r="S33" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F33:H33,M33:O33)</f>
-        <v>2.5075760411404297E-3</v>
+        <v>3.2057412961949655E-3</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
@@ -2449,15 +2449,15 @@
       </c>
       <c r="M34" s="23">
         <f t="array" aca="1" ref="M34:O34" ca="1">_xll.nnFeedForward($K$20,A34:D34)</f>
-        <v>7.8126863670920403E-6</v>
+        <v>2.0306650713111709E-5</v>
       </c>
       <c r="N34" s="23">
         <f ca="1"/>
-        <v>2.5397680242720201E-3</v>
+        <v>9.558603618905653E-3</v>
       </c>
       <c r="O34" s="23">
         <f ca="1"/>
-        <v>0.9974524192893609</v>
+        <v>0.99042108973038123</v>
       </c>
       <c r="P34" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -2473,7 +2473,7 @@
       </c>
       <c r="S34" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F34:H34,M34:O34)</f>
-        <v>2.5508313163382745E-3</v>
+        <v>9.625083124260532E-3</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
@@ -2501,15 +2501,15 @@
       </c>
       <c r="M35" s="23">
         <f t="array" aca="1" ref="M35:O35" ca="1">_xll.nnFeedForward($K$20,A35:D35)</f>
-        <v>0.99881579474449877</v>
+        <v>0.99873998931433372</v>
       </c>
       <c r="N35" s="23">
         <f ca="1"/>
-        <v>1.1813716923496566E-3</v>
+        <v>1.2571682918660935E-3</v>
       </c>
       <c r="O35" s="23">
         <f ca="1"/>
-        <v>2.8335631515652451E-6</v>
+        <v>2.8423938001628637E-6</v>
       </c>
       <c r="P35" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -2525,7 +2525,7 @@
       </c>
       <c r="S35" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F35:H35,M35:O35)</f>
-        <v>1.1849069805905336E-3</v>
+        <v>1.2608051665700165E-3</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
@@ -2553,15 +2553,15 @@
       </c>
       <c r="M36" s="23">
         <f t="array" aca="1" ref="M36:O36" ca="1">_xll.nnFeedForward($K$20,A36:D36)</f>
-        <v>0.99889642664983203</v>
+        <v>0.99883734930972867</v>
       </c>
       <c r="N36" s="23">
         <f ca="1"/>
-        <v>1.1009553538222567E-3</v>
+        <v>1.1600342704585777E-3</v>
       </c>
       <c r="O36" s="23">
         <f ca="1"/>
-        <v>2.6179963457506062E-6</v>
+        <v>2.6164198127002539E-6</v>
       </c>
       <c r="P36" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -2577,7 +2577,7 @@
       </c>
       <c r="S36" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F36:H36,M36:O36)</f>
-        <v>1.1041827356131884E-3</v>
+        <v>1.1633270929159503E-3</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
@@ -2605,15 +2605,15 @@
       </c>
       <c r="M37" s="23">
         <f t="array" aca="1" ref="M37:O37" ca="1">_xll.nnFeedForward($K$20,A37:D37)</f>
-        <v>0.99884276667531324</v>
+        <v>0.99877206182889178</v>
       </c>
       <c r="N37" s="23">
         <f ca="1"/>
-        <v>1.1544689437510325E-3</v>
+        <v>1.2251700804125295E-3</v>
       </c>
       <c r="O37" s="23">
         <f ca="1"/>
-        <v>2.7643809357232396E-6</v>
+        <v>2.7680906957351565E-6</v>
       </c>
       <c r="P37" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -2629,7 +2629,7 @@
       </c>
       <c r="S37" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F37:H37,M37:O37)</f>
-        <v>1.1579034362041128E-3</v>
+        <v>1.2286927049280883E-3</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
@@ -2657,15 +2657,15 @@
       </c>
       <c r="M38" s="23">
         <f t="array" aca="1" ref="M38:O38" ca="1">_xll.nnFeedForward($K$20,A38:D38)</f>
-        <v>9.044600575361803E-4</v>
+        <v>1.4251849134872818E-3</v>
       </c>
       <c r="N38" s="23">
         <f ca="1"/>
-        <v>0.9959565504827117</v>
+        <v>0.99637681478081508</v>
       </c>
       <c r="O38" s="23">
         <f ca="1"/>
-        <v>3.1389894597520242E-3</v>
+        <v>2.1980003056977439E-3</v>
       </c>
       <c r="P38" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -2681,7 +2681,7 @@
       </c>
       <c r="S38" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F38:H38,M38:O38)</f>
-        <v>4.0516463624354288E-3</v>
+        <v>3.6297648523788521E-3</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
@@ -2709,15 +2709,15 @@
       </c>
       <c r="M39" s="23">
         <f t="array" aca="1" ref="M39:O39" ca="1">_xll.nnFeedForward($K$20,A39:D39)</f>
-        <v>1.1079489895371496E-3</v>
+        <v>1.7203099448443704E-3</v>
       </c>
       <c r="N39" s="23">
         <f ca="1"/>
-        <v>0.99602417714832736</v>
+        <v>0.99611984092085915</v>
       </c>
       <c r="O39" s="23">
         <f ca="1"/>
-        <v>2.867873862135635E-3</v>
+        <v>2.1598491342964933E-3</v>
       </c>
       <c r="P39" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -2733,7 +2733,7 @@
       </c>
       <c r="S39" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F39:H39,M39:O39)</f>
-        <v>3.9837474468449484E-3</v>
+        <v>3.8877064259773548E-3</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
@@ -2761,15 +2761,15 @@
       </c>
       <c r="M40" s="23">
         <f t="array" aca="1" ref="M40:O40" ca="1">_xll.nnFeedForward($K$20,A40:D40)</f>
-        <v>7.7098631575985107E-6</v>
+        <v>4.3304348830393089E-5</v>
       </c>
       <c r="N40" s="23">
         <f ca="1"/>
-        <v>2.5042308078949888E-3</v>
+        <v>2.1880312279833836E-2</v>
       </c>
       <c r="O40" s="23">
         <f ca="1"/>
-        <v>0.99748805932894746</v>
+        <v>0.97807638337133573</v>
       </c>
       <c r="P40" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -2785,7 +2785,7 @@
       </c>
       <c r="S40" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F40:H40,M40:O40)</f>
-        <v>2.5151008873131081E-3</v>
+        <v>2.2167510390408651E-2</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
@@ -2813,15 +2813,15 @@
       </c>
       <c r="M41" s="23">
         <f t="array" aca="1" ref="M41:O41" ca="1">_xll.nnFeedForward($K$20,A41:D41)</f>
-        <v>0.99875111506718695</v>
+        <v>0.99860864912989111</v>
       </c>
       <c r="N41" s="23">
         <f ca="1"/>
-        <v>1.2458650268423119E-3</v>
+        <v>1.3882050928154543E-3</v>
       </c>
       <c r="O41" s="23">
         <f ca="1"/>
-        <v>3.0199059706713125E-6</v>
+        <v>3.145777293361906E-6</v>
       </c>
       <c r="P41" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -2837,7 +2837,7 @@
       </c>
       <c r="S41" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F41:H41,M41:O41)</f>
-        <v>1.2496654395104713E-3</v>
+        <v>1.3923196974875804E-3</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
@@ -2865,15 +2865,15 @@
       </c>
       <c r="M42" s="23">
         <f t="array" aca="1" ref="M42:O42" ca="1">_xll.nnFeedForward($K$20,A42:D42)</f>
-        <v>0.9987490818245035</v>
+        <v>0.99866311869972491</v>
       </c>
       <c r="N42" s="23">
         <f ca="1"/>
-        <v>1.247917918559214E-3</v>
+        <v>1.3338613140814451E-3</v>
       </c>
       <c r="O42" s="23">
         <f ca="1"/>
-        <v>3.0002569372136576E-6</v>
+        <v>3.0199861937959858E-6</v>
       </c>
       <c r="P42" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -2889,7 +2889,7 @@
       </c>
       <c r="S42" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F42:H42,M42:O42)</f>
-        <v>1.2517012267275198E-3</v>
+        <v>1.3377757233277818E-3</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
@@ -2917,15 +2917,15 @@
       </c>
       <c r="M43" s="23">
         <f t="array" aca="1" ref="M43:O43" ca="1">_xll.nnFeedForward($K$20,A43:D43)</f>
-        <v>7.4984034799970001E-4</v>
+        <v>1.2889176916893431E-3</v>
       </c>
       <c r="N43" s="23">
         <f ca="1"/>
-        <v>0.99574174504824275</v>
+        <v>0.99620668830338266</v>
       </c>
       <c r="O43" s="23">
         <f ca="1"/>
-        <v>3.5084146037576572E-3</v>
+        <v>2.5043940049279683E-3</v>
       </c>
       <c r="P43" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -2941,7 +2941,7 @@
       </c>
       <c r="S43" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F43:H43,M43:O43)</f>
-        <v>4.2673471397908997E-3</v>
+        <v>3.8005245496085869E-3</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
@@ -2969,15 +2969,15 @@
       </c>
       <c r="M44" s="23">
         <f t="array" aca="1" ref="M44:O44" ca="1">_xll.nnFeedForward($K$20,A44:D44)</f>
-        <v>0.99880396976664987</v>
+        <v>0.99870790089778805</v>
       </c>
       <c r="N44" s="23">
         <f ca="1"/>
-        <v>1.1931564301668057E-3</v>
+        <v>1.2891824264113683E-3</v>
       </c>
       <c r="O44" s="23">
         <f ca="1"/>
-        <v>2.8738031834118331E-6</v>
+        <v>2.916675800626944E-6</v>
       </c>
       <c r="P44" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -2993,7 +2993,7 @@
       </c>
       <c r="S44" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F44:H44,M44:O44)</f>
-        <v>1.1967460483241657E-3</v>
+        <v>1.2929345820162691E-3</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
@@ -3021,15 +3021,15 @@
       </c>
       <c r="M45" s="23">
         <f t="array" aca="1" ref="M45:O45" ca="1">_xll.nnFeedForward($K$20,A45:D45)</f>
-        <v>8.1062610031088402E-6</v>
+        <v>3.4784335134639059E-5</v>
       </c>
       <c r="N45" s="23">
         <f ca="1"/>
-        <v>2.6463616257823308E-3</v>
+        <v>1.7307910788038002E-2</v>
       </c>
       <c r="O45" s="23">
         <f ca="1"/>
-        <v>0.99734553211321453</v>
+        <v>0.98265730487682734</v>
       </c>
       <c r="P45" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -3045,7 +3045,7 @@
       </c>
       <c r="S45" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F45:H45,M45:O45)</f>
-        <v>2.6579972337421065E-3</v>
+        <v>1.749484130957529E-2</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
@@ -3073,15 +3073,15 @@
       </c>
       <c r="M46" s="23">
         <f t="array" aca="1" ref="M46:O46" ca="1">_xll.nnFeedForward($K$20,A46:D46)</f>
-        <v>0.99885256529270483</v>
+        <v>0.9987968901412777</v>
       </c>
       <c r="N46" s="23">
         <f ca="1"/>
-        <v>1.1447028017506982E-3</v>
+        <v>1.2003993642187712E-3</v>
       </c>
       <c r="O46" s="23">
         <f ca="1"/>
-        <v>2.7319055445229148E-6</v>
+        <v>2.7104945035092788E-6</v>
       </c>
       <c r="P46" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -3097,7 +3097,7 @@
       </c>
       <c r="S46" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F46:H46,M46:O46)</f>
-        <v>1.1480935145059797E-3</v>
+        <v>1.2038341764024844E-3</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
@@ -3125,15 +3125,15 @@
       </c>
       <c r="M47" s="23">
         <f t="array" aca="1" ref="M47:O47" ca="1">_xll.nnFeedForward($K$20,A47:D47)</f>
-        <v>0.99881579474449877</v>
+        <v>0.99873998931433372</v>
       </c>
       <c r="N47" s="23">
         <f ca="1"/>
-        <v>1.1813716923496566E-3</v>
+        <v>1.2571682918660935E-3</v>
       </c>
       <c r="O47" s="23">
         <f ca="1"/>
-        <v>2.8335631515652451E-6</v>
+        <v>2.8423938001628637E-6</v>
       </c>
       <c r="P47" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -3149,7 +3149,7 @@
       </c>
       <c r="S47" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F47:H47,M47:O47)</f>
-        <v>1.1849069805905336E-3</v>
+        <v>1.2608051665700165E-3</v>
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
@@ -3177,15 +3177,15 @@
       </c>
       <c r="M48" s="23">
         <f t="array" aca="1" ref="M48:O48" ca="1">_xll.nnFeedForward($K$20,A48:D48)</f>
-        <v>0.99887109945409003</v>
+        <v>0.99879859459931619</v>
       </c>
       <c r="N48" s="23">
         <f ca="1"/>
-        <v>1.1262063056906393E-3</v>
+        <v>1.1986988917319209E-3</v>
       </c>
       <c r="O48" s="23">
         <f ca="1"/>
-        <v>2.6942402193526612E-6</v>
+        <v>2.7065089517940059E-6</v>
       </c>
       <c r="P48" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -3201,7 +3201,7 @@
       </c>
       <c r="S48" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F48:H48,M48:O48)</f>
-        <v>1.1295382341007906E-3</v>
+        <v>1.2021276666996862E-3</v>
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
@@ -3229,15 +3229,15 @@
       </c>
       <c r="M49" s="23">
         <f t="array" aca="1" ref="M49:O49" ca="1">_xll.nnFeedForward($K$20,A49:D49)</f>
-        <v>6.3890179816482274E-4</v>
+        <v>1.144337990134291E-3</v>
       </c>
       <c r="N49" s="23">
         <f ca="1"/>
-        <v>0.99056478435130813</v>
+        <v>0.98584771567738805</v>
       </c>
       <c r="O49" s="23">
         <f ca="1"/>
-        <v>8.7963138505270412E-3</v>
+        <v>1.3007946332477561E-2</v>
       </c>
       <c r="P49" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -3253,7 +3253,7 @@
       </c>
       <c r="S49" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F49:H49,M49:O49)</f>
-        <v>9.4800092768808509E-3</v>
+        <v>1.4253382882259184E-2</v>
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
@@ -3281,15 +3281,15 @@
       </c>
       <c r="M50" s="23">
         <f t="array" aca="1" ref="M50:O50" ca="1">_xll.nnFeedForward($K$20,A50:D50)</f>
-        <v>6.4338026407660806E-4</v>
+        <v>1.0967253425594715E-3</v>
       </c>
       <c r="N50" s="23">
         <f ca="1"/>
-        <v>0.9928187128309458</v>
+        <v>0.99329612315958793</v>
       </c>
       <c r="O50" s="23">
         <f ca="1"/>
-        <v>6.5379069049774554E-3</v>
+        <v>5.6071514978526847E-3</v>
       </c>
       <c r="P50" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -3305,7 +3305,7 @@
       </c>
       <c r="S50" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F50:H50,M50:O50)</f>
-        <v>7.2071967289341543E-3</v>
+        <v>6.7264487588915315E-3</v>
       </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
@@ -3333,15 +3333,15 @@
       </c>
       <c r="M51" s="23">
         <f t="array" aca="1" ref="M51:O51" ca="1">_xll.nnFeedForward($K$20,A51:D51)</f>
-        <v>8.2300484603508553E-4</v>
+        <v>1.1682149315652276E-3</v>
       </c>
       <c r="N51" s="23">
         <f ca="1"/>
-        <v>0.99565573413281372</v>
+        <v>0.99633536505898546</v>
       </c>
       <c r="O51" s="23">
         <f ca="1"/>
-        <v>3.5212610211512179E-3</v>
+        <v>2.4964200094493134E-3</v>
       </c>
       <c r="P51" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -3357,7 +3357,7 @@
       </c>
       <c r="S51" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F51:H51,M51:O51)</f>
-        <v>4.3537296087673002E-3</v>
+        <v>3.6713661656592607E-3</v>
       </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
@@ -3385,15 +3385,15 @@
       </c>
       <c r="M52" s="23">
         <f t="array" aca="1" ref="M52:O52" ca="1">_xll.nnFeedForward($K$20,A52:D52)</f>
-        <v>1.0959032986913011E-3</v>
+        <v>1.7908687338693261E-3</v>
       </c>
       <c r="N52" s="23">
         <f ca="1"/>
-        <v>0.99606611825906688</v>
+        <v>0.99606364984907547</v>
       </c>
       <c r="O52" s="23">
         <f ca="1"/>
-        <v>2.8379784422417776E-3</v>
+        <v>2.1454814170551182E-3</v>
       </c>
       <c r="P52" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -3409,7 +3409,7 @@
       </c>
       <c r="S52" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F52:H52,M52:O52)</f>
-        <v>3.9416398066015237E-3</v>
+        <v>3.9441179684471276E-3</v>
       </c>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
@@ -3437,15 +3437,15 @@
       </c>
       <c r="M53" s="23">
         <f t="array" aca="1" ref="M53:O53" ca="1">_xll.nnFeedForward($K$20,A53:D53)</f>
-        <v>8.0222394043472499E-6</v>
+        <v>5.5228551509484281E-5</v>
       </c>
       <c r="N53" s="23">
         <f ca="1"/>
-        <v>2.618501047436239E-3</v>
+        <v>2.8493386925106255E-2</v>
       </c>
       <c r="O53" s="23">
         <f ca="1"/>
-        <v>0.99737347671315946</v>
+        <v>0.9714513845233842</v>
       </c>
       <c r="P53" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -3461,7 +3461,7 @@
       </c>
       <c r="S53" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F53:H53,M53:O53)</f>
-        <v>2.6299786508508765E-3</v>
+        <v>2.8964053080809085E-2</v>
       </c>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
@@ -3489,15 +3489,15 @@
       </c>
       <c r="M54" s="23">
         <f t="array" aca="1" ref="M54:O54" ca="1">_xll.nnFeedForward($K$20,A54:D54)</f>
-        <v>0.99857437882374078</v>
+        <v>0.99857692099338902</v>
       </c>
       <c r="N54" s="23">
         <f ca="1"/>
-        <v>1.4222040661282453E-3</v>
+        <v>1.4198601393980298E-3</v>
       </c>
       <c r="O54" s="23">
         <f ca="1"/>
-        <v>3.4171101309986209E-6</v>
+        <v>3.2188672129411898E-6</v>
       </c>
       <c r="P54" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -3513,7 +3513,7 @@
       </c>
       <c r="S54" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F54:H54,M54:O54)</f>
-        <v>1.4266383409709551E-3</v>
+        <v>1.4240925452183065E-3</v>
       </c>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
@@ -3541,15 +3541,15 @@
       </c>
       <c r="M55" s="23">
         <f t="array" aca="1" ref="M55:O55" ca="1">_xll.nnFeedForward($K$20,A55:D55)</f>
-        <v>0.99876785528950884</v>
+        <v>0.99866466489427363</v>
       </c>
       <c r="N55" s="23">
         <f ca="1"/>
-        <v>1.2291802255709478E-3</v>
+        <v>1.33231855664232E-3</v>
       </c>
       <c r="O55" s="23">
         <f ca="1"/>
-        <v>2.9644849202086357E-6</v>
+        <v>3.0165490839731131E-6</v>
       </c>
       <c r="P55" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -3565,7 +3565,7 @@
       </c>
       <c r="S55" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F55:H55,M55:O55)</f>
-        <v>1.2329044249011322E-3</v>
+        <v>1.3362274601318956E-3</v>
       </c>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
@@ -3593,15 +3593,15 @@
       </c>
       <c r="M56" s="23">
         <f t="array" aca="1" ref="M56:O56" ca="1">_xll.nnFeedForward($K$20,A56:D56)</f>
-        <v>9.4421575221003177E-4</v>
+        <v>1.4598520477098432E-3</v>
       </c>
       <c r="N56" s="23">
         <f ca="1"/>
-        <v>0.99600597836436133</v>
+        <v>0.99634245335534055</v>
       </c>
       <c r="O56" s="23">
         <f ca="1"/>
-        <v>3.0498058834287126E-3</v>
+        <v>2.1976945969496885E-3</v>
       </c>
       <c r="P56" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -3617,7 +3617,7 @@
       </c>
       <c r="S56" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F56:H56,M56:O56)</f>
-        <v>4.0020190416962323E-3</v>
+        <v>3.6642518230499111E-3</v>
       </c>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.25">
@@ -3645,15 +3645,15 @@
       </c>
       <c r="M57" s="23">
         <f t="array" aca="1" ref="M57:O57" ca="1">_xll.nnFeedForward($K$20,A57:D57)</f>
-        <v>0.99881186008905631</v>
+        <v>0.99870611151121103</v>
       </c>
       <c r="N57" s="23">
         <f ca="1"/>
-        <v>1.1852846123080231E-3</v>
+        <v>1.2909677487578472E-3</v>
       </c>
       <c r="O57" s="23">
         <f ca="1"/>
-        <v>2.8552986355534016E-6</v>
+        <v>2.9207400311059735E-6</v>
       </c>
       <c r="P57" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -3669,7 +3669,7 @@
       </c>
       <c r="S57" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F57:H57,M57:O57)</f>
-        <v>1.1888463087560662E-3</v>
+        <v>1.2947262852544624E-3</v>
       </c>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
@@ -3697,15 +3697,15 @@
       </c>
       <c r="M58" s="23">
         <f t="array" aca="1" ref="M58:O58" ca="1">_xll.nnFeedForward($K$20,A58:D58)</f>
-        <v>8.7808300531525095E-6</v>
+        <v>5.3836929333942264E-5</v>
       </c>
       <c r="N58" s="23">
         <f ca="1"/>
-        <v>2.8985005476922414E-3</v>
+        <v>2.8192535858390509E-2</v>
       </c>
       <c r="O58" s="23">
         <f ca="1"/>
-        <v>0.99709271862225457</v>
+        <v>0.97175362721227554</v>
       </c>
       <c r="P58" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -3721,7 +3721,7 @@
       </c>
       <c r="S58" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F58:H58,M58:O58)</f>
-        <v>2.9115157292089796E-3</v>
+        <v>2.8652976596852637E-2</v>
       </c>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.25">
@@ -3749,15 +3749,15 @@
       </c>
       <c r="M59" s="23">
         <f t="array" aca="1" ref="M59:O59" ca="1">_xll.nnFeedForward($K$20,A59:D59)</f>
-        <v>0.99874387538710507</v>
+        <v>0.99868246682642303</v>
       </c>
       <c r="N59" s="23">
         <f ca="1"/>
-        <v>1.2531099838361021E-3</v>
+        <v>1.3145576615613826E-3</v>
       </c>
       <c r="O59" s="23">
         <f ca="1"/>
-        <v>3.0146290588680136E-6</v>
+        <v>2.9755120155486247E-6</v>
       </c>
       <c r="P59" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -3773,7 +3773,7 @@
       </c>
       <c r="S59" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F59:H59,M59:O59)</f>
-        <v>1.2569141986978544E-3</v>
+        <v>1.3184018835286616E-3</v>
       </c>
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.25">
@@ -3801,15 +3801,15 @@
       </c>
       <c r="M60" s="23">
         <f t="array" aca="1" ref="M60:O60" ca="1">_xll.nnFeedForward($K$20,A60:D60)</f>
-        <v>7.5995449914284692E-6</v>
+        <v>3.8353333230097995E-6</v>
       </c>
       <c r="N60" s="23">
         <f ca="1"/>
-        <v>2.4656752443796741E-3</v>
+        <v>1.4328925469097515E-3</v>
       </c>
       <c r="O60" s="23">
         <f ca="1"/>
-        <v>0.99752672521062891</v>
+        <v>0.99856327211976714</v>
       </c>
       <c r="P60" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -3825,7 +3825,7 @@
       </c>
       <c r="S60" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F60:H60,M60:O60)</f>
-        <v>2.476338385916199E-3</v>
+        <v>1.437760963358558E-3</v>
       </c>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
@@ -3853,15 +3853,15 @@
       </c>
       <c r="M61" s="23">
         <f t="array" aca="1" ref="M61:O61" ca="1">_xll.nnFeedForward($K$20,A61:D61)</f>
-        <v>3.5141392729526167E-5</v>
+        <v>2.2781022638098885E-4</v>
       </c>
       <c r="N61" s="23">
         <f ca="1"/>
-        <v>1.4123923144684398E-2</v>
+        <v>0.14702774664324136</v>
       </c>
       <c r="O61" s="23">
         <f ca="1"/>
-        <v>0.98584093546258611</v>
+        <v>0.85274444313037767</v>
       </c>
       <c r="P61" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -3877,7 +3877,7 @@
       </c>
       <c r="S61" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F61:H61,M61:O61)</f>
-        <v>1.426026045372367E-2</v>
+        <v>0.15929537411578046</v>
       </c>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
@@ -3905,15 +3905,15 @@
       </c>
       <c r="M62" s="23">
         <f t="array" aca="1" ref="M62:O62" ca="1">_xll.nnFeedForward($K$20,A62:D62)</f>
-        <v>7.6791325373339153E-6</v>
+        <v>1.8432876206773033E-5</v>
       </c>
       <c r="N62" s="23">
         <f ca="1"/>
-        <v>2.4928245768242475E-3</v>
+        <v>8.577857253775514E-3</v>
       </c>
       <c r="O62" s="23">
         <f ca="1"/>
-        <v>0.9974994962906385</v>
+        <v>0.99140370987001769</v>
       </c>
       <c r="P62" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -3929,7 +3929,7 @@
       </c>
       <c r="S62" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F62:H62,M62:O62)</f>
-        <v>2.5036351900370075E-3</v>
+        <v>8.63345135100301E-3</v>
       </c>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
@@ -3957,15 +3957,15 @@
       </c>
       <c r="M63" s="23">
         <f t="array" aca="1" ref="M63:O63" ca="1">_xll.nnFeedForward($K$20,A63:D63)</f>
-        <v>7.6258382951328863E-6</v>
+        <v>4.4799414179577773E-6</v>
       </c>
       <c r="N63" s="23">
         <f ca="1"/>
-        <v>2.4741456525867382E-3</v>
+        <v>1.7151584475508679E-3</v>
       </c>
       <c r="O63" s="23">
         <f ca="1"/>
-        <v>0.9975182285091182</v>
+        <v>0.99828036161103118</v>
       </c>
       <c r="P63" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -3981,7 +3981,7 @@
       </c>
       <c r="S63" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F63:H63,M63:O63)</f>
-        <v>2.4848561904848797E-3</v>
+        <v>1.7211186643322058E-3</v>
       </c>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
@@ -4009,15 +4009,15 @@
       </c>
       <c r="M64" s="23">
         <f t="array" aca="1" ref="M64:O64" ca="1">_xll.nnFeedForward($K$20,A64:D64)</f>
-        <v>1.1405523889338029E-3</v>
+        <v>1.7662346763052351E-3</v>
       </c>
       <c r="N64" s="23">
         <f ca="1"/>
-        <v>0.99595045472332167</v>
+        <v>0.99611350869143189</v>
       </c>
       <c r="O64" s="23">
         <f ca="1"/>
-        <v>2.9089928877445615E-3</v>
+        <v>2.1202566322628927E-3</v>
       </c>
       <c r="P64" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -4033,7 +4033,7 @@
       </c>
       <c r="S64" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F64:H64,M64:O64)</f>
-        <v>4.0577668885183457E-3</v>
+        <v>3.8940633413743451E-3</v>
       </c>
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.25">
@@ -4061,15 +4061,15 @@
       </c>
       <c r="M65" s="23">
         <f t="array" aca="1" ref="M65:O65" ca="1">_xll.nnFeedForward($K$20,A65:D65)</f>
-        <v>6.5800544152535081E-4</v>
+        <v>1.2055441252375914E-3</v>
       </c>
       <c r="N65" s="23">
         <f ca="1"/>
-        <v>0.99505952556974231</v>
+        <v>0.99538386429117254</v>
       </c>
       <c r="O65" s="23">
         <f ca="1"/>
-        <v>4.2824689887322786E-3</v>
+        <v>3.410591583589897E-3</v>
       </c>
       <c r="P65" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -4085,7 +4085,7 @@
       </c>
       <c r="S65" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F65:H65,M65:O65)</f>
-        <v>4.9527189197615222E-3</v>
+        <v>4.6268229651687011E-3</v>
       </c>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
@@ -4113,15 +4113,15 @@
       </c>
       <c r="M66" s="23">
         <f t="array" aca="1" ref="M66:O66" ca="1">_xll.nnFeedForward($K$20,A66:D66)</f>
-        <v>8.9758645908943342E-6</v>
+        <v>5.8240650664128931E-5</v>
       </c>
       <c r="N66" s="23">
         <f ca="1"/>
-        <v>2.971955009780152E-3</v>
+        <v>3.0717876626901668E-2</v>
       </c>
       <c r="O66" s="23">
         <f ca="1"/>
-        <v>0.99701906912562899</v>
+        <v>0.9692238827224342</v>
       </c>
       <c r="P66" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -4137,7 +4137,7 @@
       </c>
       <c r="S66" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F66:H66,M66:O66)</f>
-        <v>2.9853826980635687E-3</v>
+        <v>3.1259648656993211E-2</v>
       </c>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
@@ -4165,15 +4165,15 @@
       </c>
       <c r="M67" s="23">
         <f t="array" aca="1" ref="M67:O67" ca="1">_xll.nnFeedForward($K$20,A67:D67)</f>
-        <v>7.6757205513796543E-6</v>
+        <v>7.3525371088694233E-6</v>
       </c>
       <c r="N67" s="23">
         <f ca="1"/>
-        <v>2.489341892711259E-3</v>
+        <v>3.0330466406252336E-3</v>
       </c>
       <c r="O67" s="23">
         <f ca="1"/>
-        <v>0.9975029823867374</v>
+        <v>0.99695960082226598</v>
       </c>
       <c r="P67" s="4">
         <f t="shared" ca="1" si="1"/>
@@ -4189,7 +4189,7 @@
       </c>
       <c r="S67" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F67:H67,M67:O67)</f>
-        <v>2.5001403611972775E-3</v>
+        <v>3.0450305812399661E-3</v>
       </c>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
@@ -4217,15 +4217,15 @@
       </c>
       <c r="M68" s="23">
         <f t="array" aca="1" ref="M68:O68" ca="1">_xll.nnFeedForward($K$20,A68:D68)</f>
-        <v>0.99868131352935541</v>
+        <v>0.99844874861285893</v>
       </c>
       <c r="N68" s="23">
         <f ca="1"/>
-        <v>1.3154863820828738E-3</v>
+        <v>1.5477381362566274E-3</v>
       </c>
       <c r="O68" s="23">
         <f ca="1"/>
-        <v>3.2000885616659275E-6</v>
+        <v>3.5132508844200758E-6</v>
       </c>
       <c r="P68" s="4">
         <f t="shared" ref="P68:P131" ca="1" si="4">IF(M68=MAX($M68:$O68),1,0)</f>
@@ -4241,7 +4241,7 @@
       </c>
       <c r="S68" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F68:H68,M68:O68)</f>
-        <v>1.3195567027748773E-3</v>
+        <v>1.5524558233241444E-3</v>
       </c>
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.25">
@@ -4269,15 +4269,15 @@
       </c>
       <c r="M69" s="23">
         <f t="array" aca="1" ref="M69:O69" ca="1">_xll.nnFeedForward($K$20,A69:D69)</f>
-        <v>0.99887395865016382</v>
+        <v>0.99880488773483234</v>
       </c>
       <c r="N69" s="23">
         <f ca="1"/>
-        <v>1.1233569128164382E-3</v>
+        <v>1.1924204045036485E-3</v>
       </c>
       <c r="O69" s="23">
         <f ca="1"/>
-        <v>2.6844370196411072E-6</v>
+        <v>2.691860664031115E-6</v>
       </c>
       <c r="P69" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -4293,7 +4293,7 @@
       </c>
       <c r="S69" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F69:H69,M69:O69)</f>
-        <v>1.1266758107278051E-3</v>
+        <v>1.1958269813316252E-3</v>
       </c>
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.25">
@@ -4321,15 +4321,15 @@
       </c>
       <c r="M70" s="23">
         <f t="array" aca="1" ref="M70:O70" ca="1">_xll.nnFeedForward($K$20,A70:D70)</f>
-        <v>7.8493256607551348E-6</v>
+        <v>1.9611380318564004E-5</v>
       </c>
       <c r="N70" s="23">
         <f ca="1"/>
-        <v>2.5542716701052767E-3</v>
+        <v>9.2055151480735266E-3</v>
       </c>
       <c r="O70" s="23">
         <f ca="1"/>
-        <v>0.99743787900423397</v>
+        <v>0.99077487347160786</v>
       </c>
       <c r="P70" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -4345,7 +4345,7 @@
       </c>
       <c r="S70" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F70:H70,M70:O70)</f>
-        <v>2.5654088448766855E-3</v>
+        <v>9.2679415274088198E-3</v>
       </c>
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.25">
@@ -4373,15 +4373,15 @@
       </c>
       <c r="M71" s="23">
         <f t="array" aca="1" ref="M71:O71" ca="1">_xll.nnFeedForward($K$20,A71:D71)</f>
-        <v>0.99889353113022661</v>
+        <v>0.99882384677628222</v>
       </c>
       <c r="N71" s="23">
         <f ca="1"/>
-        <v>1.1038326534086374E-3</v>
+        <v>1.1735054102355355E-3</v>
       </c>
       <c r="O71" s="23">
         <f ca="1"/>
-        <v>2.6362163646626211E-6</v>
+        <v>2.6478134821741096E-6</v>
       </c>
       <c r="P71" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -4397,7 +4397,7 @@
       </c>
       <c r="S71" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F71:H71,M71:O71)</f>
-        <v>1.1070814583684439E-3</v>
+        <v>1.1768454347379903E-3</v>
       </c>
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
@@ -4425,15 +4425,15 @@
       </c>
       <c r="M72" s="23">
         <f t="array" aca="1" ref="M72:O72" ca="1">_xll.nnFeedForward($K$20,A72:D72)</f>
-        <v>0.99879913562734812</v>
+        <v>0.99867953304660773</v>
       </c>
       <c r="N72" s="23">
         <f ca="1"/>
-        <v>1.1979689889081207E-3</v>
+        <v>1.3174847181960108E-3</v>
       </c>
       <c r="O72" s="23">
         <f ca="1"/>
-        <v>2.8953837437508433E-6</v>
+        <v>2.9822351962211537E-6</v>
       </c>
       <c r="P72" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -4449,7 +4449,7 @@
       </c>
       <c r="S72" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F72:H72,M72:O72)</f>
-        <v>1.2015859880386184E-3</v>
+        <v>1.32133953811055E-3</v>
       </c>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.25">
@@ -4477,15 +4477,15 @@
       </c>
       <c r="M73" s="23">
         <f t="array" aca="1" ref="M73:O73" ca="1">_xll.nnFeedForward($K$20,A73:D73)</f>
-        <v>7.2119217681723365E-4</v>
+        <v>1.0842793209390824E-3</v>
       </c>
       <c r="N73" s="23">
         <f ca="1"/>
-        <v>0.97352756789021277</v>
+        <v>0.94012096950166524</v>
       </c>
       <c r="O73" s="23">
         <f ca="1"/>
-        <v>2.5751239932970092E-2</v>
+        <v>5.879475117739566E-2</v>
       </c>
       <c r="P73" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -4501,7 +4501,7 @@
       </c>
       <c r="S73" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F73:H73,M73:O73)</f>
-        <v>2.6829136244991156E-2</v>
+        <v>6.1746721038840262E-2</v>
       </c>
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.25">
@@ -4529,15 +4529,15 @@
       </c>
       <c r="M74" s="23">
         <f t="array" aca="1" ref="M74:O74" ca="1">_xll.nnFeedForward($K$20,A74:D74)</f>
-        <v>8.0174271565898729E-4</v>
+        <v>1.0259751461768759E-3</v>
       </c>
       <c r="N74" s="23">
         <f ca="1"/>
-        <v>0.94903648291296983</v>
+        <v>0.83244739126226397</v>
       </c>
       <c r="O74" s="23">
         <f ca="1"/>
-        <v>5.0161774371371232E-2</v>
+        <v>0.16652663359155914</v>
       </c>
       <c r="P74" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -4553,7 +4553,7 @@
       </c>
       <c r="S74" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F74:H74,M74:O74)</f>
-        <v>5.2308037577981831E-2</v>
+        <v>0.183385252803305</v>
       </c>
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.25">
@@ -4581,15 +4581,15 @@
       </c>
       <c r="M75" s="23">
         <f t="array" aca="1" ref="M75:O75" ca="1">_xll.nnFeedForward($K$20,A75:D75)</f>
-        <v>8.1283853815807255E-4</v>
+        <v>1.3074181283972651E-3</v>
       </c>
       <c r="N75" s="23">
         <f ca="1"/>
-        <v>0.99582040497149105</v>
+        <v>0.99632308286183291</v>
       </c>
       <c r="O75" s="23">
         <f ca="1"/>
-        <v>3.3667564903507902E-3</v>
+        <v>2.3694990097698288E-3</v>
       </c>
       <c r="P75" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -4605,7 +4605,7 @@
       </c>
       <c r="S75" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F75:H75,M75:O75)</f>
-        <v>4.1883539501599209E-3</v>
+        <v>3.6836936141143813E-3</v>
       </c>
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.25">
@@ -4633,15 +4633,15 @@
       </c>
       <c r="M76" s="23">
         <f t="array" aca="1" ref="M76:O76" ca="1">_xll.nnFeedForward($K$20,A76:D76)</f>
-        <v>0.99885588006938775</v>
+        <v>0.99878151356830236</v>
       </c>
       <c r="N76" s="23">
         <f ca="1"/>
-        <v>1.1413869987380604E-3</v>
+        <v>1.2157402858672898E-3</v>
       </c>
       <c r="O76" s="23">
         <f ca="1"/>
-        <v>2.7329318742765579E-6</v>
+        <v>2.7461458304473434E-6</v>
       </c>
       <c r="P76" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -4657,7 +4657,7 @@
       </c>
       <c r="S76" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F76:H76,M76:O76)</f>
-        <v>1.1447749354704698E-3</v>
+        <v>1.2192293898740498E-3</v>
       </c>
     </row>
     <row r="77" spans="1:19" x14ac:dyDescent="0.25">
@@ -4685,15 +4685,15 @@
       </c>
       <c r="M77" s="23">
         <f t="array" aca="1" ref="M77:O77" ca="1">_xll.nnFeedForward($K$20,A77:D77)</f>
-        <v>6.3856571584029167E-4</v>
+        <v>1.1254239898062692E-3</v>
       </c>
       <c r="N77" s="23">
         <f ca="1"/>
-        <v>0.98897956206817994</v>
+        <v>0.97981419988111584</v>
       </c>
       <c r="O77" s="23">
         <f ca="1"/>
-        <v>1.038187221597979E-2</v>
+        <v>1.906037612907777E-2</v>
       </c>
       <c r="P77" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -4709,7 +4709,7 @@
       </c>
       <c r="S77" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F77:H77,M77:O77)</f>
-        <v>1.1081612822519427E-2</v>
+        <v>2.0392317250391742E-2</v>
       </c>
     </row>
     <row r="78" spans="1:19" x14ac:dyDescent="0.25">
@@ -4737,15 +4737,15 @@
       </c>
       <c r="M78" s="23">
         <f t="array" aca="1" ref="M78:O78" ca="1">_xll.nnFeedForward($K$20,A78:D78)</f>
-        <v>8.2435495664867468E-4</v>
+        <v>1.2933456349924996E-3</v>
       </c>
       <c r="N78" s="23">
         <f ca="1"/>
-        <v>0.9957616440416619</v>
+        <v>0.99650664505308428</v>
       </c>
       <c r="O78" s="23">
         <f ca="1"/>
-        <v>3.4140010016895385E-3</v>
+        <v>2.2000093119232227E-3</v>
       </c>
       <c r="P78" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -4761,7 +4761,7 @@
       </c>
       <c r="S78" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F78:H78,M78:O78)</f>
-        <v>4.2473632486975501E-3</v>
+        <v>3.4994709590633866E-3</v>
       </c>
     </row>
     <row r="79" spans="1:19" x14ac:dyDescent="0.25">
@@ -4789,15 +4789,15 @@
       </c>
       <c r="M79" s="23">
         <f t="array" aca="1" ref="M79:O79" ca="1">_xll.nnFeedForward($K$20,A79:D79)</f>
-        <v>7.677989530208508E-4</v>
+        <v>1.3540180809046949E-3</v>
       </c>
       <c r="N79" s="23">
         <f ca="1"/>
-        <v>0.99593387590291593</v>
+        <v>0.99635867515003385</v>
       </c>
       <c r="O79" s="23">
         <f ca="1"/>
-        <v>3.2983251440630605E-3</v>
+        <v>2.2873067690615469E-3</v>
       </c>
       <c r="P79" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -4813,7 +4813,7 @@
       </c>
       <c r="S79" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F79:H79,M79:O79)</f>
-        <v>4.07441325713645E-3</v>
+        <v>3.6479706111194297E-3</v>
       </c>
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.25">
@@ -4841,15 +4841,15 @@
       </c>
       <c r="M80" s="23">
         <f t="array" aca="1" ref="M80:O80" ca="1">_xll.nnFeedForward($K$20,A80:D80)</f>
-        <v>7.025527663093536E-4</v>
+        <v>6.6126966016606344E-4</v>
       </c>
       <c r="N80" s="23">
         <f ca="1"/>
-        <v>0.48751396767233562</v>
+        <v>0.51639226294321239</v>
       </c>
       <c r="O80" s="23">
         <f ca="1"/>
-        <v>0.51178347956135495</v>
+        <v>0.4829464673966215</v>
       </c>
       <c r="P80" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -4857,15 +4857,15 @@
       </c>
       <c r="Q80" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R80" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S80" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F80:H80,M80:O80)</f>
-        <v>0.71843633731912515</v>
+        <v>0.66088860280350925</v>
       </c>
     </row>
     <row r="81" spans="1:19" x14ac:dyDescent="0.25">
@@ -4893,15 +4893,15 @@
       </c>
       <c r="M81" s="23">
         <f t="array" aca="1" ref="M81:O81" ca="1">_xll.nnFeedForward($K$20,A81:D81)</f>
-        <v>8.4829781347770807E-4</v>
+        <v>1.3270821386476401E-3</v>
       </c>
       <c r="N81" s="23">
         <f ca="1"/>
-        <v>0.99583925709989429</v>
+        <v>0.99644923441431665</v>
       </c>
       <c r="O81" s="23">
         <f ca="1"/>
-        <v>3.312445086628021E-3</v>
+        <v>2.2236834470356079E-3</v>
       </c>
       <c r="P81" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -4917,7 +4917,7 @@
       </c>
       <c r="S81" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F81:H81,M81:O81)</f>
-        <v>4.1694228759780972E-3</v>
+        <v>3.557084516267526E-3</v>
       </c>
     </row>
     <row r="82" spans="1:19" x14ac:dyDescent="0.25">
@@ -4945,15 +4945,15 @@
       </c>
       <c r="M82" s="23">
         <f t="array" aca="1" ref="M82:O82" ca="1">_xll.nnFeedForward($K$20,A82:D82)</f>
-        <v>7.8126863670920403E-6</v>
+        <v>2.0306650713111709E-5</v>
       </c>
       <c r="N82" s="23">
         <f ca="1"/>
-        <v>2.5397680242720201E-3</v>
+        <v>9.558603618905653E-3</v>
       </c>
       <c r="O82" s="23">
         <f ca="1"/>
-        <v>0.9974524192893609</v>
+        <v>0.99042108973038123</v>
       </c>
       <c r="P82" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -4969,7 +4969,7 @@
       </c>
       <c r="S82" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F82:H82,M82:O82)</f>
-        <v>2.5508313163382745E-3</v>
+        <v>9.625083124260532E-3</v>
       </c>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.25">
@@ -4997,15 +4997,15 @@
       </c>
       <c r="M83" s="23">
         <f t="array" aca="1" ref="M83:O83" ca="1">_xll.nnFeedForward($K$20,A83:D83)</f>
-        <v>8.7686942821630525E-4</v>
+        <v>8.5989033191188587E-4</v>
       </c>
       <c r="N83" s="23">
         <f ca="1"/>
-        <v>0.70612076406326463</v>
+        <v>0.71521255731097755</v>
       </c>
       <c r="O83" s="23">
         <f ca="1"/>
-        <v>0.29300236650851902</v>
+        <v>0.28392755235711042</v>
       </c>
       <c r="P83" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -5021,7 +5021,7 @@
       </c>
       <c r="S83" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F83:H83,M83:O83)</f>
-        <v>0.34796900220297505</v>
+        <v>0.33517549751553444</v>
       </c>
     </row>
     <row r="84" spans="1:19" x14ac:dyDescent="0.25">
@@ -5049,15 +5049,15 @@
       </c>
       <c r="M84" s="23">
         <f t="array" aca="1" ref="M84:O84" ca="1">_xll.nnFeedForward($K$20,A84:D84)</f>
-        <v>0.99876674166717716</v>
+        <v>0.99869062565018718</v>
       </c>
       <c r="N84" s="23">
         <f ca="1"/>
-        <v>1.2303031266293473E-3</v>
+        <v>1.3064178176395774E-3</v>
       </c>
       <c r="O84" s="23">
         <f ca="1"/>
-        <v>2.9552061935310732E-6</v>
+        <v>2.9565321731403056E-6</v>
       </c>
       <c r="P84" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -5073,7 +5073,7 @@
       </c>
       <c r="S84" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F84:H84,M84:O84)</f>
-        <v>1.2340194216910552E-3</v>
+        <v>1.3102323294329095E-3</v>
       </c>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.25">
@@ -5101,15 +5101,15 @@
       </c>
       <c r="M85" s="23">
         <f t="array" aca="1" ref="M85:O85" ca="1">_xll.nnFeedForward($K$20,A85:D85)</f>
-        <v>6.7647385581021883E-4</v>
+        <v>1.1451736256365593E-3</v>
       </c>
       <c r="N85" s="23">
         <f ca="1"/>
-        <v>0.98298584514460663</v>
+        <v>0.94805734826318055</v>
       </c>
       <c r="O85" s="23">
         <f ca="1"/>
-        <v>1.6337680999583219E-2</v>
+        <v>5.0797478111182889E-2</v>
       </c>
       <c r="P85" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -5125,7 +5125,7 @@
       </c>
       <c r="S85" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F85:H85,M85:O85)</f>
-        <v>1.7160558588080192E-2</v>
+        <v>5.3340284608297664E-2</v>
       </c>
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.25">
@@ -5153,15 +5153,15 @@
       </c>
       <c r="M86" s="23">
         <f t="array" aca="1" ref="M86:O86" ca="1">_xll.nnFeedForward($K$20,A86:D86)</f>
-        <v>1.1241993452192905E-5</v>
+        <v>7.8900594583161278E-5</v>
       </c>
       <c r="N86" s="23">
         <f ca="1"/>
-        <v>3.8444324520492514E-3</v>
+        <v>4.401408566702341E-2</v>
       </c>
       <c r="O86" s="23">
         <f ca="1"/>
-        <v>0.9961443255544985</v>
+        <v>0.95590701373839337</v>
       </c>
       <c r="P86" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -5177,7 +5177,7 @@
       </c>
       <c r="S86" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F86:H86,M86:O86)</f>
-        <v>3.8631267200803154E-3</v>
+        <v>4.5094636625400066E-2</v>
       </c>
     </row>
     <row r="87" spans="1:19" x14ac:dyDescent="0.25">
@@ -5205,15 +5205,15 @@
       </c>
       <c r="M87" s="23">
         <f t="array" aca="1" ref="M87:O87" ca="1">_xll.nnFeedForward($K$20,A87:D87)</f>
-        <v>0.99881579474449877</v>
+        <v>0.99873998931433372</v>
       </c>
       <c r="N87" s="23">
         <f ca="1"/>
-        <v>1.1813716923496566E-3</v>
+        <v>1.2571682918660935E-3</v>
       </c>
       <c r="O87" s="23">
         <f ca="1"/>
-        <v>2.8335631515652451E-6</v>
+        <v>2.8423938001628637E-6</v>
       </c>
       <c r="P87" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -5229,7 +5229,7 @@
       </c>
       <c r="S87" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F87:H87,M87:O87)</f>
-        <v>1.1849069805905336E-3</v>
+        <v>1.2608051665700165E-3</v>
       </c>
     </row>
     <row r="88" spans="1:19" x14ac:dyDescent="0.25">
@@ -5257,15 +5257,15 @@
       </c>
       <c r="M88" s="23">
         <f t="array" aca="1" ref="M88:O88" ca="1">_xll.nnFeedForward($K$20,A88:D88)</f>
-        <v>8.489038874535621E-6</v>
+        <v>5.5585105143376255E-5</v>
       </c>
       <c r="N88" s="23">
         <f ca="1"/>
-        <v>2.7923739924152892E-3</v>
+        <v>2.8995753125557602E-2</v>
       </c>
       <c r="O88" s="23">
         <f ca="1"/>
-        <v>0.99719913696871021</v>
+        <v>0.97094866176929906</v>
       </c>
       <c r="P88" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -5281,7 +5281,7 @@
       </c>
       <c r="S88" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F88:H88,M88:O88)</f>
-        <v>2.8047927876713066E-3</v>
+        <v>2.9481683592885801E-2</v>
       </c>
     </row>
     <row r="89" spans="1:19" x14ac:dyDescent="0.25">
@@ -5309,15 +5309,15 @@
       </c>
       <c r="M89" s="23">
         <f t="array" aca="1" ref="M89:O89" ca="1">_xll.nnFeedForward($K$20,A89:D89)</f>
-        <v>1.9390819887667106E-5</v>
+        <v>1.6218498666831612E-4</v>
       </c>
       <c r="N89" s="23">
         <f ca="1"/>
-        <v>7.1760586774942906E-3</v>
+        <v>9.6139784901741035E-2</v>
       </c>
       <c r="O89" s="23">
         <f ca="1"/>
-        <v>0.99280455050261796</v>
+        <v>0.90369803011159078</v>
       </c>
       <c r="P89" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -5333,7 +5333,7 @@
       </c>
       <c r="S89" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F89:H89,M89:O89)</f>
-        <v>7.2214615983981767E-3</v>
+        <v>0.10126001188008751</v>
       </c>
     </row>
     <row r="90" spans="1:19" x14ac:dyDescent="0.25">
@@ -5361,15 +5361,15 @@
       </c>
       <c r="M90" s="23">
         <f t="array" aca="1" ref="M90:O90" ca="1">_xll.nnFeedForward($K$20,A90:D90)</f>
-        <v>7.9105214811683234E-6</v>
+        <v>3.3269572402056983E-5</v>
       </c>
       <c r="N90" s="23">
         <f ca="1"/>
-        <v>2.5753611323221137E-3</v>
+        <v>1.6472036992807408E-2</v>
       </c>
       <c r="O90" s="23">
         <f ca="1"/>
-        <v>0.99741672834619666</v>
+        <v>0.98349469343479057</v>
       </c>
       <c r="P90" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -5385,7 +5385,7 @@
       </c>
       <c r="S90" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F90:H90,M90:O90)</f>
-        <v>2.586614057487344E-3</v>
+        <v>1.6643036760064994E-2</v>
       </c>
     </row>
     <row r="91" spans="1:19" x14ac:dyDescent="0.25">
@@ -5413,15 +5413,15 @@
       </c>
       <c r="M91" s="23">
         <f t="array" aca="1" ref="M91:O91" ca="1">_xll.nnFeedForward($K$20,A91:D91)</f>
-        <v>7.6323910490810077E-6</v>
+        <v>5.6960452572784285E-6</v>
       </c>
       <c r="N91" s="23">
         <f ca="1"/>
-        <v>2.4764791757524566E-3</v>
+        <v>2.2625631861901115E-3</v>
       </c>
       <c r="O91" s="23">
         <f ca="1"/>
-        <v>0.99751588843319849</v>
+        <v>0.99773174076855264</v>
       </c>
       <c r="P91" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -5437,7 +5437,7 @@
       </c>
       <c r="S91" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F91:H91,M91:O91)</f>
-        <v>2.4872020911387415E-3</v>
+        <v>2.2708356281122039E-3</v>
       </c>
     </row>
     <row r="92" spans="1:19" x14ac:dyDescent="0.25">
@@ -5465,15 +5465,15 @@
       </c>
       <c r="M92" s="23">
         <f t="array" aca="1" ref="M92:O92" ca="1">_xll.nnFeedForward($K$20,A92:D92)</f>
-        <v>0.99885015336728222</v>
+        <v>0.99878772288308093</v>
       </c>
       <c r="N92" s="23">
         <f ca="1"/>
-        <v>1.1471085884942123E-3</v>
+        <v>1.2095455557778515E-3</v>
       </c>
       <c r="O92" s="23">
         <f ca="1"/>
-        <v>2.7380442235693903E-6</v>
+        <v>2.7315611412430686E-6</v>
       </c>
       <c r="P92" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -5489,7 +5489,7 @@
       </c>
       <c r="S92" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F92:H92,M92:O92)</f>
-        <v>1.1505082135501161E-3</v>
+        <v>1.2130125192241774E-3</v>
       </c>
     </row>
     <row r="93" spans="1:19" x14ac:dyDescent="0.25">
@@ -5517,15 +5517,15 @@
       </c>
       <c r="M93" s="23">
         <f t="array" aca="1" ref="M93:O93" ca="1">_xll.nnFeedForward($K$20,A93:D93)</f>
-        <v>7.9792956741561787E-6</v>
+        <v>6.4860821416910008E-5</v>
       </c>
       <c r="N93" s="23">
         <f ca="1"/>
-        <v>2.6026488582564615E-3</v>
+        <v>3.3655909536572125E-2</v>
       </c>
       <c r="O93" s="23">
         <f ca="1"/>
-        <v>0.99738937184606946</v>
+        <v>0.96627922964201096</v>
       </c>
       <c r="P93" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -5541,7 +5541,7 @@
       </c>
       <c r="S93" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F93:H93,M93:O93)</f>
-        <v>2.6140417860533176E-3</v>
+        <v>3.4302428938292891E-2</v>
       </c>
     </row>
     <row r="94" spans="1:19" x14ac:dyDescent="0.25">
@@ -5569,15 +5569,15 @@
       </c>
       <c r="M94" s="23">
         <f t="array" aca="1" ref="M94:O94" ca="1">_xll.nnFeedForward($K$20,A94:D94)</f>
-        <v>0.99886975643542431</v>
+        <v>0.99880264793511697</v>
       </c>
       <c r="N94" s="23">
         <f ca="1"/>
-        <v>1.1275500128267095E-3</v>
+        <v>1.19465497741044E-3</v>
       </c>
       <c r="O94" s="23">
         <f ca="1"/>
-        <v>2.6935517491158217E-6</v>
+        <v>2.6970874725425554E-6</v>
       </c>
       <c r="P94" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -5593,7 +5593,7 @@
       </c>
       <c r="S94" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F94:H94,M94:O94)</f>
-        <v>1.1308827715184077E-3</v>
+        <v>1.1980694635763814E-3</v>
       </c>
     </row>
     <row r="95" spans="1:19" x14ac:dyDescent="0.25">
@@ -5621,15 +5621,15 @@
       </c>
       <c r="M95" s="23">
         <f t="array" aca="1" ref="M95:O95" ca="1">_xll.nnFeedForward($K$20,A95:D95)</f>
-        <v>6.7070238649543474E-4</v>
+        <v>1.2097823159944185E-3</v>
       </c>
       <c r="N95" s="23">
         <f ca="1"/>
-        <v>0.99482514701246827</v>
+        <v>0.99438669817406122</v>
       </c>
       <c r="O95" s="23">
         <f ca="1"/>
-        <v>4.5041506010363962E-3</v>
+        <v>4.4035195099443357E-3</v>
       </c>
       <c r="P95" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -5645,7 +5645,7 @@
       </c>
       <c r="S95" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F95:H95,M95:O95)</f>
-        <v>5.1882889119196736E-3</v>
+        <v>5.6291156107634854E-3</v>
       </c>
     </row>
     <row r="96" spans="1:19" x14ac:dyDescent="0.25">
@@ -5673,15 +5673,15 @@
       </c>
       <c r="M96" s="23">
         <f t="array" aca="1" ref="M96:O96" ca="1">_xll.nnFeedForward($K$20,A96:D96)</f>
-        <v>8.2477243248149667E-4</v>
+        <v>9.5510337672335402E-4</v>
       </c>
       <c r="N96" s="23">
         <f ca="1"/>
-        <v>0.94122560653905663</v>
+        <v>0.94510405936867581</v>
       </c>
       <c r="O96" s="23">
         <f ca="1"/>
-        <v>5.794962102846183E-2</v>
+        <v>5.394083725460086E-2</v>
       </c>
       <c r="P96" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -5697,7 +5697,7 @@
       </c>
       <c r="S96" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F96:H96,M96:O96)</f>
-        <v>6.0572416231422448E-2</v>
+        <v>5.6460241816638237E-2</v>
       </c>
     </row>
     <row r="97" spans="1:19" x14ac:dyDescent="0.25">
@@ -5725,15 +5725,15 @@
       </c>
       <c r="M97" s="23">
         <f t="array" aca="1" ref="M97:O97" ca="1">_xll.nnFeedForward($K$20,A97:D97)</f>
-        <v>7.2637051001321997E-4</v>
+        <v>1.2803801116470599E-3</v>
       </c>
       <c r="N97" s="23">
         <f ca="1"/>
-        <v>0.9957309984200724</v>
+        <v>0.99619451890972899</v>
       </c>
       <c r="O97" s="23">
         <f ca="1"/>
-        <v>3.5426310699143708E-3</v>
+        <v>2.5251009786238917E-3</v>
       </c>
       <c r="P97" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -5749,7 +5749,7 @@
       </c>
       <c r="S97" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F97:H97,M97:O97)</f>
-        <v>4.2781397837833484E-3</v>
+        <v>3.8127403559529774E-3</v>
       </c>
     </row>
     <row r="98" spans="1:19" x14ac:dyDescent="0.25">
@@ -5777,15 +5777,15 @@
       </c>
       <c r="M98" s="23">
         <f t="array" aca="1" ref="M98:O98" ca="1">_xll.nnFeedForward($K$20,A98:D98)</f>
-        <v>0.99874985436331831</v>
+        <v>0.99868071758836441</v>
       </c>
       <c r="N98" s="23">
         <f ca="1"/>
-        <v>1.2471495174581806E-3</v>
+        <v>1.3163029534620822E-3</v>
       </c>
       <c r="O98" s="23">
         <f ca="1"/>
-        <v>2.9961192234879367E-6</v>
+        <v>2.9794581734259765E-6</v>
       </c>
       <c r="P98" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -5801,7 +5801,7 @@
       </c>
       <c r="S98" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F98:H98,M98:O98)</f>
-        <v>1.2509277206186427E-3</v>
+        <v>1.3201534308409115E-3</v>
       </c>
     </row>
     <row r="99" spans="1:19" x14ac:dyDescent="0.25">
@@ -5829,15 +5829,15 @@
       </c>
       <c r="M99" s="23">
         <f t="array" aca="1" ref="M99:O99" ca="1">_xll.nnFeedForward($K$20,A99:D99)</f>
-        <v>6.57790272069673E-4</v>
+        <v>1.1385207063538984E-3</v>
       </c>
       <c r="N99" s="23">
         <f ca="1"/>
-        <v>0.99379616327177878</v>
+        <v>0.9934571288230073</v>
       </c>
       <c r="O99" s="23">
         <f ca="1"/>
-        <v>5.5460464561515955E-3</v>
+        <v>5.404350470638801E-3</v>
       </c>
       <c r="P99" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -5853,7 +5853,7 @@
       </c>
       <c r="S99" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F99:H99,M99:O99)</f>
-        <v>6.2231604857093661E-3</v>
+        <v>6.5643695841262088E-3</v>
       </c>
     </row>
     <row r="100" spans="1:19" x14ac:dyDescent="0.25">
@@ -5881,15 +5881,15 @@
       </c>
       <c r="M100" s="23">
         <f t="array" aca="1" ref="M100:O100" ca="1">_xll.nnFeedForward($K$20,A100:D100)</f>
-        <v>0.9988781770215337</v>
+        <v>0.99881242470634912</v>
       </c>
       <c r="N100" s="23">
         <f ca="1"/>
-        <v>1.1191510805355796E-3</v>
+        <v>1.1849008946523401E-3</v>
       </c>
       <c r="O100" s="23">
         <f ca="1"/>
-        <v>2.671897930709408E-6</v>
+        <v>2.6743989985603692E-6</v>
       </c>
       <c r="P100" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -5905,7 +5905,7 @@
       </c>
       <c r="S100" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F100:H100,M100:O100)</f>
-        <v>1.1224526928599145E-3</v>
+        <v>1.1882810199806883E-3</v>
       </c>
     </row>
     <row r="101" spans="1:19" x14ac:dyDescent="0.25">
@@ -5933,15 +5933,15 @@
       </c>
       <c r="M101" s="23">
         <f t="array" aca="1" ref="M101:O101" ca="1">_xll.nnFeedForward($K$20,A101:D101)</f>
-        <v>6.4602963351885099E-4</v>
+        <v>1.1115725219377046E-3</v>
       </c>
       <c r="N101" s="23">
         <f ca="1"/>
-        <v>0.99153914879368354</v>
+        <v>0.99085451667579527</v>
       </c>
       <c r="O101" s="23">
         <f ca="1"/>
-        <v>7.8148215727974167E-3</v>
+        <v>8.0339108022669248E-3</v>
       </c>
       <c r="P101" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -5957,7 +5957,7 @@
       </c>
       <c r="S101" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F101:H101,M101:O101)</f>
-        <v>8.4968473905966662E-3</v>
+        <v>9.187559994286356E-3</v>
       </c>
     </row>
     <row r="102" spans="1:19" x14ac:dyDescent="0.25">
@@ -5985,15 +5985,15 @@
       </c>
       <c r="M102" s="23">
         <f t="array" aca="1" ref="M102:O102" ca="1">_xll.nnFeedForward($K$20,A102:D102)</f>
-        <v>0.99882956680743007</v>
+        <v>0.9987475155977914</v>
       </c>
       <c r="N102" s="23">
         <f ca="1"/>
-        <v>1.1676269087628546E-3</v>
+        <v>1.2496593649887113E-3</v>
       </c>
       <c r="O102" s="23">
         <f ca="1"/>
-        <v>2.8062838070985975E-6</v>
+        <v>2.825037219949552E-6</v>
       </c>
       <c r="P102" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -6009,7 +6009,7 @@
       </c>
       <c r="S102" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F102:H102,M102:O102)</f>
-        <v>1.171118684432888E-3</v>
+        <v>1.2532694163445868E-3</v>
       </c>
     </row>
     <row r="103" spans="1:19" x14ac:dyDescent="0.25">
@@ -6037,15 +6037,15 @@
       </c>
       <c r="M103" s="23">
         <f t="array" aca="1" ref="M103:O103" ca="1">_xll.nnFeedForward($K$20,A103:D103)</f>
-        <v>7.896169436960922E-6</v>
+        <v>8.5461667952097622E-6</v>
       </c>
       <c r="N103" s="23">
         <f ca="1"/>
-        <v>2.5679146399686941E-3</v>
+        <v>3.6054156225833805E-3</v>
       </c>
       <c r="O103" s="23">
         <f ca="1"/>
-        <v>0.99742418919059428</v>
+        <v>0.99638603821062144</v>
       </c>
       <c r="P103" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -6061,7 +6061,7 @@
       </c>
       <c r="S103" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F103:H103,M103:O103)</f>
-        <v>2.5791339177608447E-3</v>
+        <v>3.6205079257028254E-3</v>
       </c>
     </row>
     <row r="104" spans="1:19" x14ac:dyDescent="0.25">
@@ -6089,15 +6089,15 @@
       </c>
       <c r="M104" s="23">
         <f t="array" aca="1" ref="M104:O104" ca="1">_xll.nnFeedForward($K$20,A104:D104)</f>
-        <v>0.99882858816424702</v>
+        <v>0.99873602470558676</v>
       </c>
       <c r="N104" s="23">
         <f ca="1"/>
-        <v>1.1686025987996188E-3</v>
+        <v>1.2611237439819675E-3</v>
       </c>
       <c r="O104" s="23">
         <f ca="1"/>
-        <v>2.8092369533791174E-6</v>
+        <v>2.8515504312438864E-6</v>
       </c>
       <c r="P104" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -6113,7 +6113,7 @@
       </c>
       <c r="S104" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F104:H104,M104:O104)</f>
-        <v>1.1720984748746228E-3</v>
+        <v>1.264774784947552E-3</v>
       </c>
     </row>
     <row r="105" spans="1:19" x14ac:dyDescent="0.25">
@@ -6141,15 +6141,15 @@
       </c>
       <c r="M105" s="23">
         <f t="array" aca="1" ref="M105:O105" ca="1">_xll.nnFeedForward($K$20,A105:D105)</f>
-        <v>7.1505208858659583E-4</v>
+        <v>1.2154956774643282E-3</v>
       </c>
       <c r="N105" s="23">
         <f ca="1"/>
-        <v>0.99536823402259389</v>
+        <v>0.99608727743657455</v>
       </c>
       <c r="O105" s="23">
         <f ca="1"/>
-        <v>3.9167138888195202E-3</v>
+        <v>2.6972268859612432E-3</v>
       </c>
       <c r="P105" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -6165,7 +6165,7 @@
       </c>
       <c r="S105" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F105:H105,M105:O105)</f>
-        <v>4.6425258430832428E-3</v>
+        <v>3.9203972882751927E-3</v>
       </c>
     </row>
     <row r="106" spans="1:19" x14ac:dyDescent="0.25">
@@ -6193,15 +6193,15 @@
       </c>
       <c r="M106" s="23">
         <f t="array" aca="1" ref="M106:O106" ca="1">_xll.nnFeedForward($K$20,A106:D106)</f>
-        <v>7.3958417799237111E-4</v>
+        <v>1.1497199776427205E-3</v>
       </c>
       <c r="N106" s="23">
         <f ca="1"/>
-        <v>0.99520448455434085</v>
+        <v>0.99557177379877115</v>
       </c>
       <c r="O106" s="23">
         <f ca="1"/>
-        <v>4.0559312676668752E-3</v>
+        <v>3.2785062235860503E-3</v>
       </c>
       <c r="P106" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -6217,7 +6217,7 @@
       </c>
       <c r="S106" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F106:H106,M106:O106)</f>
-        <v>4.8070508233507038E-3</v>
+        <v>4.4380598359843176E-3</v>
       </c>
     </row>
     <row r="107" spans="1:19" x14ac:dyDescent="0.25">
@@ -6245,15 +6245,15 @@
       </c>
       <c r="M107" s="23">
         <f t="array" aca="1" ref="M107:O107" ca="1">_xll.nnFeedForward($K$20,A107:D107)</f>
-        <v>9.2965737813341181E-4</v>
+        <v>1.4106890934182865E-3</v>
       </c>
       <c r="N107" s="23">
         <f ca="1"/>
-        <v>0.99590555251264734</v>
+        <v>0.99640156557021464</v>
       </c>
       <c r="O107" s="23">
         <f ca="1"/>
-        <v>3.1647901092191847E-3</v>
+        <v>2.1877453363670966E-3</v>
       </c>
       <c r="P107" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -6269,7 +6269,7 @@
       </c>
       <c r="S107" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F107:H107,M107:O107)</f>
-        <v>4.1028526884143331E-3</v>
+        <v>3.6049243687155592E-3</v>
       </c>
     </row>
     <row r="108" spans="1:19" x14ac:dyDescent="0.25">
@@ -6297,15 +6297,15 @@
       </c>
       <c r="M108" s="23">
         <f t="array" aca="1" ref="M108:O108" ca="1">_xll.nnFeedForward($K$20,A108:D108)</f>
-        <v>9.7280633280219433E-6</v>
+        <v>6.5514557769421019E-5</v>
       </c>
       <c r="N108" s="23">
         <f ca="1"/>
-        <v>3.2532523616848599E-3</v>
+        <v>3.5407223427392227E-2</v>
       </c>
       <c r="O108" s="23">
         <f ca="1"/>
-        <v>0.99673701957498706</v>
+        <v>0.9645272620148384</v>
       </c>
       <c r="P108" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -6321,7 +6321,7 @@
       </c>
       <c r="S108" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F108:H108,M108:O108)</f>
-        <v>3.2683155544163994E-3</v>
+        <v>3.6117181597929982E-2</v>
       </c>
     </row>
     <row r="109" spans="1:19" x14ac:dyDescent="0.25">
@@ -6349,15 +6349,15 @@
       </c>
       <c r="M109" s="23">
         <f t="array" aca="1" ref="M109:O109" ca="1">_xll.nnFeedForward($K$20,A109:D109)</f>
-        <v>8.2214143195808733E-4</v>
+        <v>1.3289654630503779E-3</v>
       </c>
       <c r="N109" s="23">
         <f ca="1"/>
-        <v>0.99588652746141704</v>
+        <v>0.99633067353894711</v>
       </c>
       <c r="O109" s="23">
         <f ca="1"/>
-        <v>3.2913311066248944E-3</v>
+        <v>2.34036099800258E-3</v>
       </c>
       <c r="P109" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -6373,7 +6373,7 @@
       </c>
       <c r="S109" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F109:H109,M109:O109)</f>
-        <v>4.1219561394443523E-3</v>
+        <v>3.6760749527289258E-3</v>
       </c>
     </row>
     <row r="110" spans="1:19" x14ac:dyDescent="0.25">
@@ -6401,15 +6401,15 @@
       </c>
       <c r="M110" s="23">
         <f t="array" aca="1" ref="M110:O110" ca="1">_xll.nnFeedForward($K$20,A110:D110)</f>
-        <v>8.8726130714159338E-4</v>
+        <v>1.3512870402249927E-3</v>
       </c>
       <c r="N110" s="23">
         <f ca="1"/>
-        <v>0.99583871571680327</v>
+        <v>0.9964753533652887</v>
       </c>
       <c r="O110" s="23">
         <f ca="1"/>
-        <v>3.274022976055059E-3</v>
+        <v>2.1733595944862464E-3</v>
       </c>
       <c r="P110" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -6425,7 +6425,7 @@
       </c>
       <c r="S110" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F110:H110,M110:O110)</f>
-        <v>4.1699665211842128E-3</v>
+        <v>3.5308728360728043E-3</v>
       </c>
     </row>
     <row r="111" spans="1:19" x14ac:dyDescent="0.25">
@@ -6453,15 +6453,15 @@
       </c>
       <c r="M111" s="23">
         <f t="array" aca="1" ref="M111:O111" ca="1">_xll.nnFeedForward($K$20,A111:D111)</f>
-        <v>1.4268060377759803E-3</v>
+        <v>2.0661266930728827E-3</v>
       </c>
       <c r="N111" s="23">
         <f ca="1"/>
-        <v>0.9958066711871556</v>
+        <v>0.99583279854775653</v>
       </c>
       <c r="O111" s="23">
         <f ca="1"/>
-        <v>2.7665227750684569E-3</v>
+        <v>2.1010747591706366E-3</v>
       </c>
       <c r="P111" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -6477,7 +6477,7 @@
       </c>
       <c r="S111" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F111:H111,M111:O111)</f>
-        <v>4.202145472177338E-3</v>
+        <v>4.1759084337981969E-3</v>
       </c>
     </row>
     <row r="112" spans="1:19" x14ac:dyDescent="0.25">
@@ -6505,15 +6505,15 @@
       </c>
       <c r="M112" s="23">
         <f t="array" aca="1" ref="M112:O112" ca="1">_xll.nnFeedForward($K$20,A112:D112)</f>
-        <v>6.203597998601098E-4</v>
+        <v>1.1136725640168443E-3</v>
       </c>
       <c r="N112" s="23">
         <f ca="1"/>
-        <v>0.99287736480861488</v>
+        <v>0.99205877211097804</v>
       </c>
       <c r="O112" s="23">
         <f ca="1"/>
-        <v>6.5022753915250165E-3</v>
+        <v>6.8275553250051763E-3</v>
       </c>
       <c r="P112" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -6529,7 +6529,7 @@
       </c>
       <c r="S112" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F112:H112,M112:O112)</f>
-        <v>7.1481222528886005E-3</v>
+        <v>7.9729273726289601E-3</v>
       </c>
     </row>
     <row r="113" spans="1:19" x14ac:dyDescent="0.25">
@@ -6557,15 +6557,15 @@
       </c>
       <c r="M113" s="23">
         <f t="array" aca="1" ref="M113:O113" ca="1">_xll.nnFeedForward($K$20,A113:D113)</f>
-        <v>1.994102101587549E-5</v>
+        <v>1.537033721082533E-4</v>
       </c>
       <c r="N113" s="23">
         <f ca="1"/>
-        <v>7.3808793049894086E-3</v>
+        <v>9.5361576504390269E-2</v>
       </c>
       <c r="O113" s="23">
         <f ca="1"/>
-        <v>0.9925991796739948</v>
+        <v>0.90448472012350145</v>
       </c>
       <c r="P113" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -6581,7 +6581,7 @@
       </c>
       <c r="S113" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F113:H113,M113:O113)</f>
-        <v>7.4283422708117074E-3</v>
+        <v>0.10038986746415905</v>
       </c>
     </row>
     <row r="114" spans="1:19" x14ac:dyDescent="0.25">
@@ -6609,15 +6609,15 @@
       </c>
       <c r="M114" s="23">
         <f t="array" aca="1" ref="M114:O114" ca="1">_xll.nnFeedForward($K$20,A114:D114)</f>
-        <v>7.988042787527189E-6</v>
+        <v>2.9002736547614411E-5</v>
       </c>
       <c r="N114" s="23">
         <f ca="1"/>
-        <v>2.6021077675225323E-3</v>
+        <v>1.4220808185308199E-2</v>
       </c>
       <c r="O114" s="23">
         <f ca="1"/>
-        <v>0.99738990418968998</v>
+        <v>0.98575018907814416</v>
       </c>
       <c r="P114" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -6633,7 +6633,7 @@
       </c>
       <c r="S114" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F114:H114,M114:O114)</f>
-        <v>2.6135080491863734E-3</v>
+        <v>1.4352314412961463E-2</v>
       </c>
     </row>
     <row r="115" spans="1:19" x14ac:dyDescent="0.25">
@@ -6661,15 +6661,15 @@
       </c>
       <c r="M115" s="23">
         <f t="array" aca="1" ref="M115:O115" ca="1">_xll.nnFeedForward($K$20,A115:D115)</f>
-        <v>7.1840536048084708E-5</v>
+        <v>3.1722109594556136E-4</v>
       </c>
       <c r="N115" s="23">
         <f ca="1"/>
-        <v>3.2063935546402245E-2</v>
+        <v>0.21729385790831809</v>
       </c>
       <c r="O115" s="23">
         <f ca="1"/>
-        <v>0.96786422391754967</v>
+        <v>0.78238892099573631</v>
       </c>
       <c r="P115" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -6685,7 +6685,7 @@
       </c>
       <c r="S115" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F115:H115,M115:O115)</f>
-        <v>3.2663466091537585E-2</v>
+        <v>0.24540332064331033</v>
       </c>
     </row>
     <row r="116" spans="1:19" x14ac:dyDescent="0.25">
@@ -6713,15 +6713,15 @@
       </c>
       <c r="M116" s="23">
         <f t="array" aca="1" ref="M116:O116" ca="1">_xll.nnFeedForward($K$20,A116:D116)</f>
-        <v>7.9342369765841283E-4</v>
+        <v>1.3027915056724642E-3</v>
       </c>
       <c r="N116" s="23">
         <f ca="1"/>
-        <v>0.99580303383349711</v>
+        <v>0.9963995213221728</v>
       </c>
       <c r="O116" s="23">
         <f ca="1"/>
-        <v>3.4035424688445286E-3</v>
+        <v>2.2976871721548217E-3</v>
       </c>
       <c r="P116" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -6737,7 +6737,7 @@
       </c>
       <c r="S116" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F116:H116,M116:O116)</f>
-        <v>4.2057981493553278E-3</v>
+        <v>3.6069760015205498E-3</v>
       </c>
     </row>
     <row r="117" spans="1:19" x14ac:dyDescent="0.25">
@@ -6765,15 +6765,15 @@
       </c>
       <c r="M117" s="23">
         <f t="array" aca="1" ref="M117:O117" ca="1">_xll.nnFeedForward($K$20,A117:D117)</f>
-        <v>0.99887850615686491</v>
+        <v>0.99880498691287656</v>
       </c>
       <c r="N117" s="23">
         <f ca="1"/>
-        <v>1.1188184857453118E-3</v>
+        <v>1.1923214838143999E-3</v>
       </c>
       <c r="O117" s="23">
         <f ca="1"/>
-        <v>2.675357389889962E-6</v>
+        <v>2.6916033090827736E-6</v>
       </c>
       <c r="P117" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -6789,7 +6789,7 @@
       </c>
       <c r="S117" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F117:H117,M117:O117)</f>
-        <v>1.1221231879367341E-3</v>
+        <v>1.1957276846216117E-3</v>
       </c>
     </row>
     <row r="118" spans="1:19" x14ac:dyDescent="0.25">
@@ -6817,15 +6817,15 @@
       </c>
       <c r="M118" s="23">
         <f t="array" aca="1" ref="M118:O118" ca="1">_xll.nnFeedForward($K$20,A118:D118)</f>
-        <v>7.9030525469835952E-6</v>
+        <v>1.1809914790938392E-5</v>
       </c>
       <c r="N118" s="23">
         <f ca="1"/>
-        <v>2.5698666398664594E-3</v>
+        <v>5.2090145090439612E-3</v>
       </c>
       <c r="O118" s="23">
         <f ca="1"/>
-        <v>0.99742223030758659</v>
+        <v>0.99477917557616513</v>
       </c>
       <c r="P118" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -6841,7 +6841,7 @@
       </c>
       <c r="S118" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F118:H118,M118:O118)</f>
-        <v>2.5810978614394606E-3</v>
+        <v>5.2345005488661665E-3</v>
       </c>
     </row>
     <row r="119" spans="1:19" x14ac:dyDescent="0.25">
@@ -6869,15 +6869,15 @@
       </c>
       <c r="M119" s="23">
         <f t="array" aca="1" ref="M119:O119" ca="1">_xll.nnFeedForward($K$20,A119:D119)</f>
-        <v>0.99882578857155402</v>
+        <v>0.99875862036520402</v>
       </c>
       <c r="N119" s="23">
         <f ca="1"/>
-        <v>1.171406323319619E-3</v>
+        <v>1.238580438458354E-3</v>
       </c>
       <c r="O119" s="23">
         <f ca="1"/>
-        <v>2.8051051263934309E-6</v>
+        <v>2.7991963375938599E-6</v>
       </c>
       <c r="P119" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -6893,7 +6893,7 @@
       </c>
       <c r="S119" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F119:H119,M119:O119)</f>
-        <v>1.1749013548178289E-3</v>
+        <v>1.2421507847541228E-3</v>
       </c>
     </row>
     <row r="120" spans="1:19" x14ac:dyDescent="0.25">
@@ -6921,15 +6921,15 @@
       </c>
       <c r="M120" s="23">
         <f t="array" aca="1" ref="M120:O120" ca="1">_xll.nnFeedForward($K$20,A120:D120)</f>
-        <v>7.5324958980168188E-4</v>
+        <v>1.2814349608542511E-3</v>
       </c>
       <c r="N120" s="23">
         <f ca="1"/>
-        <v>0.9957052880880809</v>
+        <v>0.99636853281888738</v>
       </c>
       <c r="O120" s="23">
         <f ca="1"/>
-        <v>3.5414623221174711E-3</v>
+        <v>2.3500322202584813E-3</v>
       </c>
       <c r="P120" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -6945,7 +6945,7 @@
       </c>
       <c r="S120" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F120:H120,M120:O120)</f>
-        <v>4.3039606771426951E-3</v>
+        <v>3.6380769650506757E-3</v>
       </c>
     </row>
     <row r="121" spans="1:19" x14ac:dyDescent="0.25">
@@ -6973,15 +6973,15 @@
       </c>
       <c r="M121" s="23">
         <f t="array" aca="1" ref="M121:O121" ca="1">_xll.nnFeedForward($K$20,A121:D121)</f>
-        <v>7.9104624369719724E-6</v>
+        <v>2.7698981314663631E-5</v>
       </c>
       <c r="N121" s="23">
         <f ca="1"/>
-        <v>2.575178760133892E-3</v>
+        <v>1.3507335165446581E-2</v>
       </c>
       <c r="O121" s="23">
         <f ca="1"/>
-        <v>0.99741691077742911</v>
+        <v>0.98646496585323862</v>
       </c>
       <c r="P121" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -6997,7 +6997,7 @@
       </c>
       <c r="S121" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F121:H121,M121:O121)</f>
-        <v>2.5864311537816156E-3</v>
+        <v>1.3627467730181765E-2</v>
       </c>
     </row>
     <row r="122" spans="1:19" x14ac:dyDescent="0.25">
@@ -7025,15 +7025,15 @@
       </c>
       <c r="M122" s="23">
         <f t="array" aca="1" ref="M122:O122" ca="1">_xll.nnFeedForward($K$20,A122:D122)</f>
-        <v>0.9988227976699684</v>
+        <v>0.99875974900569808</v>
       </c>
       <c r="N122" s="23">
         <f ca="1"/>
-        <v>1.1743930910451982E-3</v>
+        <v>1.2374544727399423E-3</v>
       </c>
       <c r="O122" s="23">
         <f ca="1"/>
-        <v>2.8092389864181208E-6</v>
+        <v>2.7965215619970111E-6</v>
       </c>
       <c r="P122" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -7049,7 +7049,7 @@
       </c>
       <c r="S122" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F122:H122,M122:O122)</f>
-        <v>1.1778957769661702E-3</v>
+        <v>1.2410207420858103E-3</v>
       </c>
     </row>
     <row r="123" spans="1:19" x14ac:dyDescent="0.25">
@@ -7077,15 +7077,15 @@
       </c>
       <c r="M123" s="23">
         <f t="array" aca="1" ref="M123:O123" ca="1">_xll.nnFeedForward($K$20,A123:D123)</f>
-        <v>0.9988054559632944</v>
+        <v>0.99872864271754169</v>
       </c>
       <c r="N123" s="23">
         <f ca="1"/>
-        <v>1.1916864577889638E-3</v>
+        <v>1.2684887397269007E-3</v>
       </c>
       <c r="O123" s="23">
         <f ca="1"/>
-        <v>2.8575789165595933E-6</v>
+        <v>2.8685427314169683E-6</v>
       </c>
       <c r="P123" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -7101,7 +7101,7 @@
       </c>
       <c r="S123" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F123:H123,M123:O123)</f>
-        <v>1.19525807312202E-3</v>
+        <v>1.2721661427677834E-3</v>
       </c>
     </row>
     <row r="124" spans="1:19" x14ac:dyDescent="0.25">
@@ -7129,15 +7129,15 @@
       </c>
       <c r="M124" s="23">
         <f t="array" aca="1" ref="M124:O124" ca="1">_xll.nnFeedForward($K$20,A124:D124)</f>
-        <v>2.3203691618416873E-3</v>
+        <v>3.1620620740104638E-3</v>
       </c>
       <c r="N124" s="23">
         <f ca="1"/>
-        <v>0.99507075936687461</v>
+        <v>0.99475156485991179</v>
       </c>
       <c r="O124" s="23">
         <f ca="1"/>
-        <v>2.6088714712836393E-3</v>
+        <v>2.0863730660777781E-3</v>
       </c>
       <c r="P124" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -7153,7 +7153,7 @@
       </c>
       <c r="S124" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F124:H124,M124:O124)</f>
-        <v>4.9414294105093364E-3</v>
+        <v>5.262256557550974E-3</v>
       </c>
     </row>
     <row r="125" spans="1:19" x14ac:dyDescent="0.25">
@@ -7181,15 +7181,15 @@
       </c>
       <c r="M125" s="23">
         <f t="array" aca="1" ref="M125:O125" ca="1">_xll.nnFeedForward($K$20,A125:D125)</f>
-        <v>0.99889725845319255</v>
+        <v>0.99884040576956501</v>
       </c>
       <c r="N125" s="23">
         <f ca="1"/>
-        <v>1.1001308993007775E-3</v>
+        <v>1.1569849479311515E-3</v>
       </c>
       <c r="O125" s="23">
         <f ca="1"/>
-        <v>2.6106475066662175E-6</v>
+        <v>2.6092825038256499E-6</v>
       </c>
       <c r="P125" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -7205,7 +7205,7 @@
       </c>
       <c r="S125" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F125:H125,M125:O125)</f>
-        <v>1.1033500136292055E-3</v>
+        <v>1.1602670800299202E-3</v>
       </c>
     </row>
     <row r="126" spans="1:19" x14ac:dyDescent="0.25">
@@ -7233,15 +7233,15 @@
       </c>
       <c r="M126" s="23">
         <f t="array" aca="1" ref="M126:O126" ca="1">_xll.nnFeedForward($K$20,A126:D126)</f>
-        <v>7.6739993310552434E-6</v>
+        <v>7.378078643481835E-6</v>
       </c>
       <c r="N126" s="23">
         <f ca="1"/>
-        <v>2.4905519958913669E-3</v>
+        <v>3.0445690004594593E-3</v>
       </c>
       <c r="O126" s="23">
         <f ca="1"/>
-        <v>0.99750177400477769</v>
+        <v>0.99694805292089705</v>
       </c>
       <c r="P126" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -7257,7 +7257,7 @@
       </c>
       <c r="S126" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F126:H126,M126:O126)</f>
-        <v>2.5013517687950239E-3</v>
+        <v>3.0566137669982177E-3</v>
       </c>
     </row>
     <row r="127" spans="1:19" x14ac:dyDescent="0.25">
@@ -7285,15 +7285,15 @@
       </c>
       <c r="M127" s="23">
         <f t="array" aca="1" ref="M127:O127" ca="1">_xll.nnFeedForward($K$20,A127:D127)</f>
-        <v>7.9426102864445841E-6</v>
+        <v>4.6664470690738196E-5</v>
       </c>
       <c r="N127" s="23">
         <f ca="1"/>
-        <v>2.5877659906587153E-3</v>
+        <v>2.3772490996845624E-2</v>
       </c>
       <c r="O127" s="23">
         <f ca="1"/>
-        <v>0.99740429139905484</v>
+        <v>0.97618084453246357</v>
       </c>
       <c r="P127" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -7309,7 +7309,7 @@
       </c>
       <c r="S127" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F127:H127,M127:O127)</f>
-        <v>2.5990832935931111E-3</v>
+        <v>2.4107418204236227E-2</v>
       </c>
     </row>
     <row r="128" spans="1:19" x14ac:dyDescent="0.25">
@@ -7337,15 +7337,15 @@
       </c>
       <c r="M128" s="23">
         <f t="array" aca="1" ref="M128:O128" ca="1">_xll.nnFeedForward($K$20,A128:D128)</f>
-        <v>7.7306531734707451E-6</v>
+        <v>8.2276703424808252E-6</v>
       </c>
       <c r="N128" s="23">
         <f ca="1"/>
-        <v>2.5097018134592249E-3</v>
+        <v>3.4480239720580054E-3</v>
       </c>
       <c r="O128" s="23">
         <f ca="1"/>
-        <v>0.99748256753336728</v>
+        <v>0.99654374835759951</v>
       </c>
       <c r="P128" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -7361,7 +7361,7 @@
       </c>
       <c r="S128" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F128:H128,M128:O128)</f>
-        <v>2.5206065278536235E-3</v>
+        <v>3.462238278302093E-3</v>
       </c>
     </row>
     <row r="129" spans="1:19" x14ac:dyDescent="0.25">
@@ -7389,15 +7389,15 @@
       </c>
       <c r="M129" s="23">
         <f t="array" aca="1" ref="M129:O129" ca="1">_xll.nnFeedForward($K$20,A129:D129)</f>
-        <v>0.99886669600826727</v>
+        <v>0.99879395184275699</v>
       </c>
       <c r="N129" s="23">
         <f ca="1"/>
-        <v>1.1305981871156728E-3</v>
+        <v>1.2033308701398606E-3</v>
       </c>
       <c r="O129" s="23">
         <f ca="1"/>
-        <v>2.7058046170513053E-6</v>
+        <v>2.7172871031968154E-6</v>
       </c>
       <c r="P129" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -7413,7 +7413,7 @@
       </c>
       <c r="S129" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F129:H129,M129:O129)</f>
-        <v>1.1339466663112267E-3</v>
+        <v>1.206776018604564E-3</v>
       </c>
     </row>
     <row r="130" spans="1:19" x14ac:dyDescent="0.25">
@@ -7441,15 +7441,15 @@
       </c>
       <c r="M130" s="23">
         <f t="array" aca="1" ref="M130:O130" ca="1">_xll.nnFeedForward($K$20,A130:D130)</f>
-        <v>7.5858989205884958E-4</v>
+        <v>1.042736400446175E-3</v>
       </c>
       <c r="N130" s="23">
         <f ca="1"/>
-        <v>0.96865899024507984</v>
+        <v>0.95635220668343013</v>
       </c>
       <c r="O130" s="23">
         <f ca="1"/>
-        <v>3.0582419862861431E-2</v>
+        <v>4.2605056916123644E-2</v>
       </c>
       <c r="P130" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -7465,7 +7465,7 @@
       </c>
       <c r="S130" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F130:H130,M130:O130)</f>
-        <v>3.1842648281206178E-2</v>
+        <v>4.4629016746750176E-2</v>
       </c>
     </row>
     <row r="131" spans="1:19" x14ac:dyDescent="0.25">
@@ -7493,15 +7493,15 @@
       </c>
       <c r="M131" s="23">
         <f t="array" aca="1" ref="M131:O131" ca="1">_xll.nnFeedForward($K$20,A131:D131)</f>
-        <v>7.6474477806980254E-6</v>
+        <v>1.272153641473035E-5</v>
       </c>
       <c r="N131" s="23">
         <f ca="1"/>
-        <v>2.4829234396426892E-3</v>
+        <v>5.6564478250887874E-3</v>
       </c>
       <c r="O131" s="23">
         <f ca="1"/>
-        <v>0.99750942911257667</v>
+        <v>0.99433083063849648</v>
       </c>
       <c r="P131" s="4">
         <f t="shared" ca="1" si="4"/>
@@ -7517,7 +7517,7 @@
       </c>
       <c r="S131" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F131:H131,M131:O131)</f>
-        <v>2.4936775183576699E-3</v>
+        <v>5.68530009626234E-3</v>
       </c>
     </row>
     <row r="132" spans="1:19" x14ac:dyDescent="0.25">
@@ -7545,15 +7545,15 @@
       </c>
       <c r="M132" s="23">
         <f t="array" aca="1" ref="M132:O132" ca="1">_xll.nnFeedForward($K$20,A132:D132)</f>
-        <v>0.99887384343364705</v>
+        <v>0.99880962775709048</v>
       </c>
       <c r="N132" s="23">
         <f ca="1"/>
-        <v>1.1234748497399056E-3</v>
+        <v>1.187691347036577E-3</v>
       </c>
       <c r="O132" s="23">
         <f ca="1"/>
-        <v>2.6817166130112538E-6</v>
+        <v>2.6808958728703182E-6</v>
       </c>
       <c r="P132" s="4">
         <f t="shared" ref="P132:P152" ca="1" si="7">IF(M132=MAX($M132:$O132),1,0)</f>
@@ -7569,7 +7569,7 @@
       </c>
       <c r="S132" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F132:H132,M132:O132)</f>
-        <v>1.126791157136047E-3</v>
+        <v>1.1910812986972712E-3</v>
       </c>
     </row>
     <row r="133" spans="1:19" x14ac:dyDescent="0.25">
@@ -7597,15 +7597,15 @@
       </c>
       <c r="M133" s="23">
         <f t="array" aca="1" ref="M133:O133" ca="1">_xll.nnFeedForward($K$20,A133:D133)</f>
-        <v>7.8413444103664508E-6</v>
+        <v>1.6228524552507314E-5</v>
       </c>
       <c r="N133" s="23">
         <f ca="1"/>
-        <v>2.5494111680309309E-3</v>
+        <v>7.4491410949001314E-3</v>
       </c>
       <c r="O133" s="23">
         <f ca="1"/>
-        <v>0.99744274748755868</v>
+        <v>0.99253463038054746</v>
       </c>
       <c r="P133" s="4">
         <f t="shared" ca="1" si="7"/>
@@ -7621,7 +7621,7 @@
       </c>
       <c r="S133" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F133:H133,M133:O133)</f>
-        <v>2.5605278677795482E-3</v>
+        <v>7.4933749584251662E-3</v>
       </c>
     </row>
     <row r="134" spans="1:19" x14ac:dyDescent="0.25">
@@ -7649,15 +7649,15 @@
       </c>
       <c r="M134" s="23">
         <f t="array" aca="1" ref="M134:O134" ca="1">_xll.nnFeedForward($K$20,A134:D134)</f>
-        <v>0.99886070888049472</v>
+        <v>0.99876771394837449</v>
       </c>
       <c r="N134" s="23">
         <f ca="1"/>
-        <v>1.1365553403072937E-3</v>
+        <v>1.2295078480419664E-3</v>
       </c>
       <c r="O134" s="23">
         <f ca="1"/>
-        <v>2.7357791979037244E-6</v>
+        <v>2.7782035836105336E-6</v>
       </c>
       <c r="P134" s="4">
         <f t="shared" ca="1" si="7"/>
@@ -7673,7 +7673,7 @@
       </c>
       <c r="S134" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F134:H134,M134:O134)</f>
-        <v>1.1399406049816597E-3</v>
+        <v>1.2330459404130748E-3</v>
       </c>
     </row>
     <row r="135" spans="1:19" x14ac:dyDescent="0.25">
@@ -7701,15 +7701,15 @@
       </c>
       <c r="M135" s="23">
         <f t="array" aca="1" ref="M135:O135" ca="1">_xll.nnFeedForward($K$20,A135:D135)</f>
-        <v>0.99879449411188637</v>
+        <v>0.99873254603054884</v>
       </c>
       <c r="N135" s="23">
         <f ca="1"/>
-        <v>1.2026234278325395E-3</v>
+        <v>1.2645943265413707E-3</v>
       </c>
       <c r="O135" s="23">
         <f ca="1"/>
-        <v>2.8824602810902625E-6</v>
+        <v>2.8596429098755303E-6</v>
       </c>
       <c r="P135" s="4">
         <f t="shared" ca="1" si="7"/>
@@ -7725,7 +7725,7 @@
       </c>
       <c r="S135" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F135:H135,M135:O135)</f>
-        <v>1.206233094830174E-3</v>
+        <v>1.2682578685753833E-3</v>
       </c>
     </row>
     <row r="136" spans="1:19" x14ac:dyDescent="0.25">
@@ -7753,15 +7753,15 @@
       </c>
       <c r="M136" s="23">
         <f t="array" aca="1" ref="M136:O136" ca="1">_xll.nnFeedForward($K$20,A136:D136)</f>
-        <v>0.99886136703181927</v>
+        <v>0.99879135552399512</v>
       </c>
       <c r="N136" s="23">
         <f ca="1"/>
-        <v>1.1359154583260639E-3</v>
+        <v>1.2059211400174603E-3</v>
       </c>
       <c r="O136" s="23">
         <f ca="1"/>
-        <v>2.7175098547253501E-6</v>
+        <v>2.7233359873741709E-6</v>
       </c>
       <c r="P136" s="4">
         <f t="shared" ca="1" si="7"/>
@@ -7777,7 +7777,7 @@
       </c>
       <c r="S136" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F136:H136,M136:O136)</f>
-        <v>1.1392817031929811E-3</v>
+        <v>1.209375475811521E-3</v>
       </c>
     </row>
     <row r="137" spans="1:19" x14ac:dyDescent="0.25">
@@ -7805,15 +7805,15 @@
       </c>
       <c r="M137" s="23">
         <f t="array" aca="1" ref="M137:O137" ca="1">_xll.nnFeedForward($K$20,A137:D137)</f>
-        <v>0.99886413033752097</v>
+        <v>0.9988026703052737</v>
       </c>
       <c r="N137" s="23">
         <f ca="1"/>
-        <v>1.1331640444797965E-3</v>
+        <v>1.194632639259429E-3</v>
       </c>
       <c r="O137" s="23">
         <f ca="1"/>
-        <v>2.705617999253443E-6</v>
+        <v>2.6970554670067935E-6</v>
       </c>
       <c r="P137" s="4">
         <f t="shared" ca="1" si="7"/>
@@ -7829,7 +7829,7 @@
       </c>
       <c r="S137" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F137:H137,M137:O137)</f>
-        <v>1.1365152513402681E-3</v>
+        <v>1.1980470666028424E-3</v>
       </c>
     </row>
     <row r="138" spans="1:19" x14ac:dyDescent="0.25">
@@ -7857,15 +7857,15 @@
       </c>
       <c r="M138" s="23">
         <f t="array" aca="1" ref="M138:O138" ca="1">_xll.nnFeedForward($K$20,A138:D138)</f>
-        <v>7.651247100444288E-4</v>
+        <v>1.3521930132140614E-3</v>
       </c>
       <c r="N138" s="23">
         <f ca="1"/>
-        <v>0.99595999588112627</v>
+        <v>0.99640538383642996</v>
       </c>
       <c r="O138" s="23">
         <f ca="1"/>
-        <v>3.2748794088294023E-3</v>
+        <v>2.2424231503559455E-3</v>
       </c>
       <c r="P138" s="4">
         <f t="shared" ca="1" si="7"/>
@@ -7881,7 +7881,7 @@
       </c>
       <c r="S138" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F138:H138,M138:O138)</f>
-        <v>4.0481869821507848E-3</v>
+        <v>3.6010923204416834E-3</v>
       </c>
     </row>
     <row r="139" spans="1:19" x14ac:dyDescent="0.25">
@@ -7909,15 +7909,15 @@
       </c>
       <c r="M139" s="23">
         <f t="array" aca="1" ref="M139:O139" ca="1">_xll.nnFeedForward($K$20,A139:D139)</f>
-        <v>0.99886892263994209</v>
+        <v>0.99879532886197053</v>
       </c>
       <c r="N139" s="23">
         <f ca="1"/>
-        <v>1.1283730926638384E-3</v>
+        <v>1.2019569787085264E-3</v>
       </c>
       <c r="O139" s="23">
         <f ca="1"/>
-        <v>2.7042673941419862E-6</v>
+        <v>2.7141593208502864E-6</v>
       </c>
       <c r="P139" s="4">
         <f t="shared" ca="1" si="7"/>
@@ -7933,7 +7933,7 @@
       </c>
       <c r="S139" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F139:H139,M139:O139)</f>
-        <v>1.1317175108073315E-3</v>
+        <v>1.205397337584551E-3</v>
       </c>
     </row>
     <row r="140" spans="1:19" x14ac:dyDescent="0.25">
@@ -7961,15 +7961,15 @@
       </c>
       <c r="M140" s="23">
         <f t="array" aca="1" ref="M140:O140" ca="1">_xll.nnFeedForward($K$20,A140:D140)</f>
-        <v>0.99885686118277783</v>
+        <v>0.9987850398256648</v>
       </c>
       <c r="N140" s="23">
         <f ca="1"/>
-        <v>1.1404075450553348E-3</v>
+        <v>1.2122221785063625E-3</v>
       </c>
       <c r="O140" s="23">
         <f ca="1"/>
-        <v>2.7312721669303628E-6</v>
+        <v>2.7379958288920959E-6</v>
       </c>
       <c r="P140" s="4">
         <f t="shared" ca="1" si="7"/>
@@ -7985,7 +7985,7 @@
       </c>
       <c r="S140" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F140:H140,M140:O140)</f>
-        <v>1.1437926987656359E-3</v>
+        <v>1.2156988368054143E-3</v>
       </c>
     </row>
     <row r="141" spans="1:19" x14ac:dyDescent="0.25">
@@ -8013,15 +8013,15 @@
       </c>
       <c r="M141" s="23">
         <f t="array" aca="1" ref="M141:O141" ca="1">_xll.nnFeedForward($K$20,A141:D141)</f>
-        <v>1.0538452109742632E-5</v>
+        <v>6.0533995160097081E-5</v>
       </c>
       <c r="N141" s="23">
         <f ca="1"/>
-        <v>3.5646213677572496E-3</v>
+        <v>3.2940275001209517E-2</v>
       </c>
       <c r="O141" s="23">
         <f ca="1"/>
-        <v>0.996424840180133</v>
+        <v>0.96699919100363041</v>
       </c>
       <c r="P141" s="4">
         <f t="shared" ca="1" si="7"/>
@@ -8037,7 +8037,7 @@
       </c>
       <c r="S141" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F141:H141,M141:O141)</f>
-        <v>3.5815659769838416E-3</v>
+        <v>3.3557620133504565E-2</v>
       </c>
     </row>
     <row r="142" spans="1:19" x14ac:dyDescent="0.25">
@@ -8065,15 +8065,15 @@
       </c>
       <c r="M142" s="23">
         <f t="array" aca="1" ref="M142:O142" ca="1">_xll.nnFeedForward($K$20,A142:D142)</f>
-        <v>7.7568009010105623E-6</v>
+        <v>2.7476003793093761E-5</v>
       </c>
       <c r="N142" s="23">
         <f ca="1"/>
-        <v>2.5199125422982844E-3</v>
+        <v>1.335676627216517E-2</v>
       </c>
       <c r="O142" s="23">
         <f ca="1"/>
-        <v>0.99747233065680063</v>
+        <v>0.98661575772404175</v>
       </c>
       <c r="P142" s="4">
         <f t="shared" ca="1" si="7"/>
@@ -8089,7 +8089,7 @@
       </c>
       <c r="S142" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F142:H142,M142:O142)</f>
-        <v>2.5308692927672825E-3</v>
+        <v>1.3474618564615622E-2</v>
       </c>
     </row>
     <row r="143" spans="1:19" x14ac:dyDescent="0.25">
@@ -8117,15 +8117,15 @@
       </c>
       <c r="M143" s="23">
         <f t="array" aca="1" ref="M143:O143" ca="1">_xll.nnFeedForward($K$20,A143:D143)</f>
-        <v>0.99882529578384061</v>
+        <v>0.99874644374024901</v>
       </c>
       <c r="N143" s="23">
         <f ca="1"/>
-        <v>1.1718939617170203E-3</v>
+        <v>1.250728846422819E-3</v>
       </c>
       <c r="O143" s="23">
         <f ca="1"/>
-        <v>2.810254442368047E-6</v>
+        <v>2.8274133281512253E-6</v>
       </c>
       <c r="P143" s="4">
         <f t="shared" ca="1" si="7"/>
@@ -8141,7 +8141,7 @@
       </c>
       <c r="S143" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F143:H143,M143:O143)</f>
-        <v>1.1753947219701533E-3</v>
+        <v>1.2543426186312611E-3</v>
       </c>
     </row>
     <row r="144" spans="1:19" x14ac:dyDescent="0.25">
@@ -8169,15 +8169,15 @@
       </c>
       <c r="M144" s="23">
         <f t="array" aca="1" ref="M144:O144" ca="1">_xll.nnFeedForward($K$20,A144:D144)</f>
-        <v>6.4120127198414982E-4</v>
+        <v>1.1694079875430583E-3</v>
       </c>
       <c r="N144" s="23">
         <f ca="1"/>
-        <v>0.99453159129761759</v>
+        <v>0.99455452728924942</v>
       </c>
       <c r="O144" s="23">
         <f ca="1"/>
-        <v>4.8272074303983559E-3</v>
+        <v>4.2760647232075195E-3</v>
       </c>
       <c r="P144" s="4">
         <f t="shared" ca="1" si="7"/>
@@ -8193,7 +8193,7 @@
       </c>
       <c r="S144" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F144:H144,M144:O144)</f>
-        <v>5.483415181962885E-3</v>
+        <v>5.4603533432435588E-3</v>
       </c>
     </row>
     <row r="145" spans="1:19" x14ac:dyDescent="0.25">
@@ -8221,15 +8221,15 @@
       </c>
       <c r="M145" s="23">
         <f t="array" aca="1" ref="M145:O145" ca="1">_xll.nnFeedForward($K$20,A145:D145)</f>
-        <v>6.7193543247977988E-4</v>
+        <v>1.1718225136923223E-3</v>
       </c>
       <c r="N145" s="23">
         <f ca="1"/>
-        <v>0.99481815254672534</v>
+        <v>0.99549680859462697</v>
       </c>
       <c r="O145" s="23">
         <f ca="1"/>
-        <v>4.5099120207948221E-3</v>
+        <v>3.3313688916806845E-3</v>
       </c>
       <c r="P145" s="4">
         <f t="shared" ca="1" si="7"/>
@@ -8245,7 +8245,7 @@
       </c>
       <c r="S145" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F145:H145,M145:O145)</f>
-        <v>5.1953197859909254E-3</v>
+        <v>4.5133613146400593E-3</v>
       </c>
     </row>
     <row r="146" spans="1:19" x14ac:dyDescent="0.25">
@@ -8273,15 +8273,15 @@
       </c>
       <c r="M146" s="23">
         <f t="array" aca="1" ref="M146:O146" ca="1">_xll.nnFeedForward($K$20,A146:D146)</f>
-        <v>0.99886805983600102</v>
+        <v>0.99880642857972313</v>
       </c>
       <c r="N146" s="23">
         <f ca="1"/>
-        <v>1.1292460796908433E-3</v>
+        <v>1.1908831229828761E-3</v>
       </c>
       <c r="O146" s="23">
         <f ca="1"/>
-        <v>2.6940843081298646E-6</v>
+        <v>2.6882972940218944E-6</v>
       </c>
       <c r="P146" s="4">
         <f t="shared" ca="1" si="7"/>
@@ -8297,7 +8297,7 @@
       </c>
       <c r="S146" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F146:H146,M146:O146)</f>
-        <v>1.1325812921245313E-3</v>
+        <v>1.194284293944738E-3</v>
       </c>
     </row>
     <row r="147" spans="1:19" x14ac:dyDescent="0.25">
@@ -8325,15 +8325,15 @@
       </c>
       <c r="M147" s="23">
         <f t="array" aca="1" ref="M147:O147" ca="1">_xll.nnFeedForward($K$20,A147:D147)</f>
-        <v>0.99885251757584714</v>
+        <v>0.99878167396436202</v>
       </c>
       <c r="N147" s="23">
         <f ca="1"/>
-        <v>1.1447388856040686E-3</v>
+        <v>1.2155801857607288E-3</v>
       </c>
       <c r="O147" s="23">
         <f ca="1"/>
-        <v>2.7435385487728893E-6</v>
+        <v>2.7458498772359876E-6</v>
       </c>
       <c r="P147" s="4">
         <f t="shared" ca="1" si="7"/>
@@ -8349,7 +8349,7 @@
       </c>
       <c r="S147" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F147:H147,M147:O147)</f>
-        <v>1.1481412861796831E-3</v>
+        <v>1.2190687981484339E-3</v>
       </c>
     </row>
     <row r="148" spans="1:19" x14ac:dyDescent="0.25">
@@ -8377,15 +8377,15 @@
       </c>
       <c r="M148" s="23">
         <f t="array" aca="1" ref="M148:O148" ca="1">_xll.nnFeedForward($K$20,A148:D148)</f>
-        <v>7.4730191022706182E-4</v>
+        <v>1.2282259365839902E-3</v>
       </c>
       <c r="N148" s="23">
         <f ca="1"/>
-        <v>0.99557164721158919</v>
+        <v>0.99630726800901714</v>
       </c>
       <c r="O148" s="23">
         <f ca="1"/>
-        <v>3.6810508781837704E-3</v>
+        <v>2.4645060543988552E-3</v>
       </c>
       <c r="P148" s="4">
         <f t="shared" ca="1" si="7"/>
@@ -8401,7 +8401,7 @@
       </c>
       <c r="S148" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F148:H148,M148:O148)</f>
-        <v>4.4381869862243489E-3</v>
+        <v>3.6995669574157977E-3</v>
       </c>
     </row>
     <row r="149" spans="1:19" x14ac:dyDescent="0.25">
@@ -8429,15 +8429,15 @@
       </c>
       <c r="M149" s="23">
         <f t="array" aca="1" ref="M149:O149" ca="1">_xll.nnFeedForward($K$20,A149:D149)</f>
-        <v>0.99875051631560985</v>
+        <v>0.99866653433169494</v>
       </c>
       <c r="N149" s="23">
         <f ca="1"/>
-        <v>1.2464841422486549E-3</v>
+        <v>1.3304534521482966E-3</v>
       </c>
       <c r="O149" s="23">
         <f ca="1"/>
-        <v>2.9995421416402185E-6</v>
+        <v>3.0122161568082756E-6</v>
       </c>
       <c r="P149" s="4">
         <f t="shared" ca="1" si="7"/>
@@ -8453,7 +8453,7 @@
       </c>
       <c r="S149" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F149:H149,M149:O149)</f>
-        <v>1.25026493997414E-3</v>
+        <v>1.3343555247993539E-3</v>
       </c>
     </row>
     <row r="150" spans="1:19" x14ac:dyDescent="0.25">
@@ -8481,15 +8481,15 @@
       </c>
       <c r="M150" s="23">
         <f t="array" aca="1" ref="M150:O150" ca="1">_xll.nnFeedForward($K$20,A150:D150)</f>
-        <v>7.6945161561260236E-6</v>
+        <v>1.5865773798430067E-5</v>
       </c>
       <c r="N150" s="23">
         <f ca="1"/>
-        <v>2.497336784674523E-3</v>
+        <v>7.2530915007265251E-3</v>
       </c>
       <c r="O150" s="23">
         <f ca="1"/>
-        <v>0.99749496869916932</v>
+        <v>0.99273104272547508</v>
       </c>
       <c r="P150" s="4">
         <f t="shared" ca="1" si="7"/>
@@ -8505,7 +8505,7 @@
       </c>
       <c r="S150" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F150:H150,M150:O150)</f>
-        <v>2.5081741414462928E-3</v>
+        <v>7.295504871585692E-3</v>
       </c>
     </row>
     <row r="151" spans="1:19" x14ac:dyDescent="0.25">
@@ -8533,15 +8533,15 @@
       </c>
       <c r="M151" s="23">
         <f t="array" aca="1" ref="M151:O151" ca="1">_xll.nnFeedForward($K$20,A151:D151)</f>
-        <v>9.4673748607023505E-6</v>
+        <v>7.7664627433276213E-5</v>
       </c>
       <c r="N151" s="23">
         <f ca="1"/>
-        <v>3.1596278555331503E-3</v>
+        <v>4.1676112408705439E-2</v>
       </c>
       <c r="O151" s="23">
         <f ca="1"/>
-        <v>0.99683090476960612</v>
+        <v>0.95824622296386119</v>
       </c>
       <c r="P151" s="4">
         <f t="shared" ca="1" si="7"/>
@@ -8557,7 +8557,7 @@
       </c>
       <c r="S151" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F151:H151,M151:O151)</f>
-        <v>3.1741274472122443E-3</v>
+        <v>4.2650516327089702E-2</v>
       </c>
     </row>
     <row r="152" spans="1:19" x14ac:dyDescent="0.25">
@@ -8585,15 +8585,15 @@
       </c>
       <c r="M152" s="23">
         <f t="array" aca="1" ref="M152:O152" ca="1">_xll.nnFeedForward($K$20,A152:D152)</f>
-        <v>7.6865047874084661E-6</v>
+        <v>8.8911348617274459E-6</v>
       </c>
       <c r="N152" s="23">
         <f ca="1"/>
-        <v>2.494921467083929E-3</v>
+        <v>3.7675631530374766E-3</v>
       </c>
       <c r="O152" s="23">
         <f ca="1"/>
-        <v>0.99749739202812859</v>
+        <v>0.99622354571210081</v>
       </c>
       <c r="P152" s="4">
         <f t="shared" ca="1" si="7"/>
@@ -8609,7 +8609,7 @@
       </c>
       <c r="S152" s="2">
         <f ca="1">_xll.nnGetCrossEntropyError(F152:H152,M152:O152)</f>
-        <v>2.5057447296781238E-3</v>
+        <v>3.7836030951649046E-3</v>
       </c>
     </row>
   </sheetData>
@@ -8627,8 +8627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:I34"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25:E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8738,15 +8738,15 @@
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C10" s="15">
         <f t="array" aca="1" ref="C10:C34" ca="1">_xll.nnGetWeights(D4,1)</f>
-        <v>-0.15084493434894294</v>
+        <v>-0.27673885966146855</v>
       </c>
       <c r="D10" s="15">
         <f t="array" aca="1" ref="D10:D33" ca="1">_xll.nnGetWeights(D4,2)</f>
-        <v>-0.55430685737490304</v>
+        <v>-1.5500290513340469</v>
       </c>
       <c r="E10" s="15">
         <f t="array" aca="1" ref="E10:E24" ca="1">_xll.nnGetWeights(D4,3)</f>
-        <v>-2.096318376055101</v>
+        <v>2.2577662912319938</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>21</v>
@@ -8759,15 +8759,15 @@
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C11" s="15">
         <f ca="1"/>
-        <v>0.30041609792517604</v>
+        <v>-0.58516646989018206</v>
       </c>
       <c r="D11" s="15">
         <f ca="1"/>
-        <v>-1.3388937695882124</v>
+        <v>-0.5511295854799112</v>
       </c>
       <c r="E11" s="15">
         <f ca="1"/>
-        <v>-0.81286416584070986</v>
+        <v>0.97157083367161778</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>22</v>
@@ -8780,288 +8780,288 @@
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C12" s="15">
         <f ca="1"/>
-        <v>-0.15929512013192365</v>
+        <v>1.0789264439740347</v>
       </c>
       <c r="D12" s="15">
         <f ca="1"/>
-        <v>9.6530702137706523E-2</v>
+        <v>-0.35358666614764217</v>
       </c>
       <c r="E12" s="15">
         <f ca="1"/>
-        <v>-2.8680805523649378</v>
+        <v>0.97343612930674306</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C13" s="15">
         <f ca="1"/>
-        <v>-0.3677946112782266</v>
+        <v>0.64849621230221466</v>
       </c>
       <c r="D13" s="15">
         <f ca="1"/>
-        <v>0.53739828465296913</v>
+        <v>7.0790345137027949E-2</v>
       </c>
       <c r="E13" s="15">
         <f ca="1"/>
-        <v>-0.97832410208593468</v>
+        <v>2.493191690588461</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C14" s="15">
         <f ca="1"/>
-        <v>0.45511732104751002</v>
+        <v>-3.7477394791022731E-2</v>
       </c>
       <c r="D14" s="15">
         <f ca="1"/>
-        <v>0.72564163143829929</v>
+        <v>-0.86908502196681292</v>
       </c>
       <c r="E14" s="15">
         <f ca="1"/>
-        <v>0.17454037336658315</v>
+        <v>0.35394299967975873</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C15" s="15">
         <f ca="1"/>
-        <v>0.32394001512688131</v>
+        <v>0.3214716572737934</v>
       </c>
       <c r="D15" s="15">
         <f ca="1"/>
-        <v>0.10206911396036066</v>
+        <v>-0.26899083975323634</v>
       </c>
       <c r="E15" s="15">
         <f ca="1"/>
-        <v>0.94427463296967462</v>
+        <v>-1.4798197609373345</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C16" s="15">
         <f ca="1"/>
-        <v>0.5493809035407945</v>
+        <v>0.19712060106743623</v>
       </c>
       <c r="D16" s="15">
         <f ca="1"/>
-        <v>-0.61005044506484529</v>
+        <v>-0.32679464065625841</v>
       </c>
       <c r="E16" s="15">
         <f ca="1"/>
-        <v>-1.5850386433576718</v>
+        <v>1.3370863202922532</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C17" s="15">
         <f ca="1"/>
-        <v>-1.3018905915118191</v>
+        <v>0.29488908357898586</v>
       </c>
       <c r="D17" s="15">
         <f ca="1"/>
-        <v>-0.14820124290772801</v>
+        <v>-0.1534949115935422</v>
       </c>
       <c r="E17" s="15">
         <f ca="1"/>
-        <v>1.6127504086649809</v>
+        <v>1.621448914260722</v>
       </c>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C18" s="15">
         <f ca="1"/>
-        <v>-0.25028621239564525</v>
+        <v>-0.10727569428117863</v>
       </c>
       <c r="D18" s="15">
         <f ca="1"/>
-        <v>0.92406983264365117</v>
+        <v>-0.95050496973975507</v>
       </c>
       <c r="E18" s="15">
         <f ca="1"/>
-        <v>-1.4360022042138829</v>
+        <v>-1.2527863413956291</v>
       </c>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C19" s="15">
         <f ca="1"/>
-        <v>-4.4726914268162166E-2</v>
+        <v>0.19498208885257878</v>
       </c>
       <c r="D19" s="15">
         <f ca="1"/>
-        <v>0.36657780285432273</v>
+        <v>-0.91586440820968673</v>
       </c>
       <c r="E19" s="15">
         <f ca="1"/>
-        <v>-0.43072319465883219</v>
+        <v>-0.25884981182283884</v>
       </c>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C20" s="15">
         <f ca="1"/>
-        <v>-1.4956722070755746</v>
+        <v>-1.7443784775886071</v>
       </c>
       <c r="D20" s="15">
         <f ca="1"/>
-        <v>0.83602333318629751</v>
+        <v>-0.18511720832104622</v>
       </c>
       <c r="E20" s="15">
         <f ca="1"/>
-        <v>1.2096946488873814</v>
+        <v>-1.3336435586240736</v>
       </c>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C21" s="15">
         <f ca="1"/>
-        <v>-3.2787302142131813</v>
+        <v>-3.2101423688002484</v>
       </c>
       <c r="D21" s="15">
         <f ca="1"/>
-        <v>-8.1425523170512201E-2</v>
+        <v>-0.14414874371125927</v>
       </c>
       <c r="E21" s="15">
         <f ca="1"/>
-        <v>1.2940647446436264</v>
+        <v>-1.6567812632362617</v>
       </c>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C22" s="15">
         <f ca="1"/>
-        <v>3.184668398553423</v>
+        <v>3.541308802905538</v>
       </c>
       <c r="D22" s="15">
         <f ca="1"/>
-        <v>6.8189899625348036E-2</v>
+        <v>0.15698810312945566</v>
       </c>
       <c r="E22" s="15">
         <f ca="1"/>
-        <v>1.2754543210064941</v>
+        <v>-2.1464329411783689</v>
       </c>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C23" s="15">
         <f ca="1"/>
-        <v>3.4260037810509387</v>
+        <v>3.3773562885858612</v>
       </c>
       <c r="D23" s="15">
         <f ca="1"/>
-        <v>-1.7290671729735072</v>
+        <v>0.90812785692095221</v>
       </c>
       <c r="E23" s="15">
         <f ca="1"/>
-        <v>2.2170179170167206</v>
+        <v>-1.2383043897125621</v>
       </c>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C24" s="15">
         <f ca="1"/>
-        <v>-1.9112600335274097</v>
+        <v>-2.0027689382330824</v>
       </c>
       <c r="D24" s="15">
         <f ca="1"/>
-        <v>-6.7478664362639287E-2</v>
+        <v>-1.4472021391950527</v>
       </c>
       <c r="E24" s="15">
         <f ca="1"/>
-        <v>-5.8655216758167761E-2</v>
+        <v>0.16203017391522245</v>
       </c>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C25" s="15">
         <f ca="1"/>
-        <v>-0.41065463508496081</v>
+        <v>-1.1678091769914078</v>
       </c>
       <c r="D25" s="15">
         <f ca="1"/>
-        <v>0.56993333242118505</v>
+        <v>-1.1126858550692658</v>
       </c>
       <c r="E25" s="15"/>
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C26" s="15">
         <f ca="1"/>
-        <v>3.5849680741780951E-2</v>
+        <v>-2.2735418971728012</v>
       </c>
       <c r="D26" s="15">
         <f ca="1"/>
-        <v>1.1775544931295077</v>
+        <v>-0.73352106034420017</v>
       </c>
       <c r="E26" s="15"/>
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C27" s="15">
         <f ca="1"/>
-        <v>0.56717636501023405</v>
+        <v>2.4638220864936358</v>
       </c>
       <c r="D27" s="15">
         <f ca="1"/>
-        <v>0.76149530757724271</v>
+        <v>0.82015273316916104</v>
       </c>
       <c r="E27" s="15"/>
     </row>
     <row r="28" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C28" s="15">
         <f ca="1"/>
-        <v>0.11950490740280917</v>
+        <v>2.7057861420538192</v>
       </c>
       <c r="D28" s="15">
         <f ca="1"/>
-        <v>-5.0445739131734453E-2</v>
+        <v>-1.6273434782002547</v>
       </c>
       <c r="E28" s="15"/>
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C29" s="15">
         <f ca="1"/>
-        <v>0.32528025793379978</v>
+        <v>-1.669366237862439</v>
       </c>
       <c r="D29" s="15">
         <f ca="1"/>
-        <v>0.4093846701590802</v>
+        <v>-0.358947342783139</v>
       </c>
       <c r="E29" s="15"/>
     </row>
     <row r="30" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C30" s="15">
         <f ca="1"/>
-        <v>-1.2698360524416845</v>
+        <v>-0.12821684987570905</v>
       </c>
       <c r="D30" s="15">
         <f ca="1"/>
-        <v>1.1997921657131609</v>
+        <v>-0.2970367660313914</v>
       </c>
       <c r="E30" s="15"/>
     </row>
     <row r="31" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C31" s="15">
         <f ca="1"/>
-        <v>-3.1601257849225153</v>
+        <v>-2.3863225720317471</v>
       </c>
       <c r="D31" s="15">
         <f ca="1"/>
-        <v>9.3702111543700062E-3</v>
+        <v>-0.15742999400245064</v>
       </c>
       <c r="E31" s="15"/>
     </row>
     <row r="32" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C32" s="15">
         <f ca="1"/>
-        <v>2.9649512234139133</v>
+        <v>1.0225136268480108</v>
       </c>
       <c r="D32" s="15">
         <f ca="1"/>
-        <v>1.2298788975822597</v>
+        <v>-0.63314044748707188</v>
       </c>
       <c r="E32" s="15"/>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C33" s="15">
         <f ca="1"/>
-        <v>3.1006955892370014</v>
+        <v>1.3746737117551215</v>
       </c>
       <c r="D33" s="15">
         <f ca="1"/>
-        <v>-1.0322602897708006</v>
+        <v>-0.40285845226202927</v>
       </c>
       <c r="E33" s="15"/>
     </row>
     <row r="34" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C34" s="15">
         <f ca="1"/>
-        <v>-2.0097402527909942</v>
+        <v>-1.025826113474813</v>
       </c>
       <c r="D34" s="15"/>
       <c r="E34" s="15"/>

</xml_diff>